<commit_message>
Melhorias e correções no RREO
</commit_message>
<xml_diff>
--- a/auxiliar/consorcios.xlsx
+++ b/auxiliar/consorcios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everton\Desktop\Sistemas\rptgen\auxiliar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF976A9D-F354-442E-8939-EC4839815F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1415BC83-6DCB-447D-9064-36E52169E863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{A96AC45E-B2A2-4150-B6D9-2DAA0E895429}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A96AC45E-B2A2-4150-B6D9-2DAA0E895429}"/>
   </bookViews>
   <sheets>
     <sheet name="Despesas" sheetId="1" r:id="rId1"/>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="12">
   <si>
     <t>COFRON</t>
   </si>
@@ -203,6 +203,12 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -219,12 +225,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -291,6 +291,7 @@
       <sheetName val="Valores calculados"/>
       <sheetName val="Parâmetros"/>
       <sheetName val="Valores manuais"/>
+      <sheetName val="Consórcios Despesas"/>
       <sheetName val="RREO A12 Valores Manuais"/>
       <sheetName val="RREO A3 Receitas"/>
       <sheetName val="RREO A3 Deduções"/>
@@ -655,13 +656,14 @@
       <sheetData sheetId="97" refreshError="1"/>
       <sheetData sheetId="98" refreshError="1"/>
       <sheetData sheetId="99" refreshError="1"/>
+      <sheetData sheetId="100" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF54E884-AE1C-4BA9-AAE0-247962D6BA1D}" name="ConsorcioDespesas" displayName="ConsorcioDespesas" ref="A1:K235" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF54E884-AE1C-4BA9-AAE0-247962D6BA1D}" name="ConsorcioDespesas" displayName="ConsorcioDespesas" ref="A1:K251" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{0E4E83A9-3008-4F12-867F-9127FDCBEBC7}" name="consorcio"/>
     <tableColumn id="2" xr3:uid="{AB479D49-5AA3-4445-8011-E951C1F88768}" name="data_base"/>
@@ -671,13 +673,13 @@
     <tableColumn id="6" xr3:uid="{9CA77609-93DE-499C-AC4A-5E76D6E3C576}" name="empenhado" dataCellStyle="Vírgula"/>
     <tableColumn id="7" xr3:uid="{DE1F7664-267D-403C-BAD6-C96344DAB890}" name="liquidado" dataCellStyle="Vírgula"/>
     <tableColumn id="8" xr3:uid="{AF1F5334-D9E9-4422-92C5-34E5E1858E36}" name="pago" dataCellStyle="Vírgula"/>
-    <tableColumn id="9" xr3:uid="{B83C89F5-C8DA-4821-809C-C6ED28F991C4}" name="ano" dataDxfId="0" dataCellStyle="Vírgula">
+    <tableColumn id="9" xr3:uid="{B83C89F5-C8DA-4821-809C-C6ED28F991C4}" name="ano" dataDxfId="2" dataCellStyle="Vírgula">
       <calculatedColumnFormula>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{55423AF4-0FA2-49E2-A517-EBAA323ACD45}" name="bimestre" dataDxfId="1" dataCellStyle="Vírgula">
       <calculatedColumnFormula array="1">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{77F4D398-298B-4A69-8283-FF31D5D938AD}" name="mes" dataDxfId="2" dataCellStyle="Vírgula">
+    <tableColumn id="12" xr3:uid="{77F4D398-298B-4A69-8283-FF31D5D938AD}" name="mes" dataDxfId="0" dataCellStyle="Vírgula">
       <calculatedColumnFormula>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1005,10 +1007,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:K235"/>
+  <dimension ref="A1:K251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
+      <selection activeCell="A205" sqref="A205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9948,6 +9950,614 @@
         <v>2</v>
       </c>
     </row>
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>0</v>
+      </c>
+      <c r="B236" s="4">
+        <v>45382</v>
+      </c>
+      <c r="C236">
+        <v>4</v>
+      </c>
+      <c r="D236">
+        <v>122</v>
+      </c>
+      <c r="E236" s="3">
+        <v>319011010100</v>
+      </c>
+      <c r="F236" s="2">
+        <v>895.44</v>
+      </c>
+      <c r="G236" s="2">
+        <v>895.44</v>
+      </c>
+      <c r="H236" s="2">
+        <v>895.44</v>
+      </c>
+      <c r="I236" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J236" s="1" cm="1">
+        <f t="array" ref="J236">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K236" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>0</v>
+      </c>
+      <c r="B237" s="4">
+        <v>45382</v>
+      </c>
+      <c r="C237">
+        <v>4</v>
+      </c>
+      <c r="D237">
+        <v>122</v>
+      </c>
+      <c r="E237" s="3">
+        <v>319013010100</v>
+      </c>
+      <c r="F237" s="2">
+        <v>71.64</v>
+      </c>
+      <c r="G237" s="2">
+        <v>71.64</v>
+      </c>
+      <c r="H237" s="2">
+        <v>71.64</v>
+      </c>
+      <c r="I237" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J237" s="1" cm="1">
+        <f t="array" ref="J237">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K237" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>0</v>
+      </c>
+      <c r="B238" s="4">
+        <v>45382</v>
+      </c>
+      <c r="C238">
+        <v>4</v>
+      </c>
+      <c r="D238">
+        <v>122</v>
+      </c>
+      <c r="E238" s="3">
+        <v>319013020100</v>
+      </c>
+      <c r="F238" s="2">
+        <v>188.04</v>
+      </c>
+      <c r="G238" s="2">
+        <v>188.04</v>
+      </c>
+      <c r="H238" s="2">
+        <v>188.04</v>
+      </c>
+      <c r="I238" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J238" s="1" cm="1">
+        <f t="array" ref="J238">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K238" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>0</v>
+      </c>
+      <c r="B239" s="4">
+        <v>45382</v>
+      </c>
+      <c r="C239">
+        <v>4</v>
+      </c>
+      <c r="D239">
+        <v>122</v>
+      </c>
+      <c r="E239" s="3">
+        <v>339014140000</v>
+      </c>
+      <c r="F239" s="2">
+        <v>0</v>
+      </c>
+      <c r="G239" s="2">
+        <v>0</v>
+      </c>
+      <c r="H239" s="2">
+        <v>0</v>
+      </c>
+      <c r="I239" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J239" s="1" cm="1">
+        <f t="array" ref="J239">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K239" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>0</v>
+      </c>
+      <c r="B240" s="4">
+        <v>45382</v>
+      </c>
+      <c r="C240">
+        <v>4</v>
+      </c>
+      <c r="D240">
+        <v>122</v>
+      </c>
+      <c r="E240" s="3">
+        <v>339030000000</v>
+      </c>
+      <c r="F240" s="2">
+        <v>0</v>
+      </c>
+      <c r="G240" s="2">
+        <v>0</v>
+      </c>
+      <c r="H240" s="2">
+        <v>0</v>
+      </c>
+      <c r="I240" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J240" s="1" cm="1">
+        <f t="array" ref="J240">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K240" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>0</v>
+      </c>
+      <c r="B241" s="4">
+        <v>45382</v>
+      </c>
+      <c r="C241">
+        <v>4</v>
+      </c>
+      <c r="D241">
+        <v>122</v>
+      </c>
+      <c r="E241" s="3">
+        <v>339033010000</v>
+      </c>
+      <c r="F241" s="2">
+        <v>0</v>
+      </c>
+      <c r="G241" s="2">
+        <v>0</v>
+      </c>
+      <c r="H241" s="2">
+        <v>0</v>
+      </c>
+      <c r="I241" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J241" s="1" cm="1">
+        <f t="array" ref="J241">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K241" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>0</v>
+      </c>
+      <c r="B242" s="4">
+        <v>45382</v>
+      </c>
+      <c r="C242">
+        <v>4</v>
+      </c>
+      <c r="D242">
+        <v>122</v>
+      </c>
+      <c r="E242" s="3">
+        <v>339039000000</v>
+      </c>
+      <c r="F242" s="2">
+        <v>10.81</v>
+      </c>
+      <c r="G242" s="2">
+        <v>64.16</v>
+      </c>
+      <c r="H242" s="2">
+        <v>67.489999999999995</v>
+      </c>
+      <c r="I242" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J242" s="1" cm="1">
+        <f t="array" ref="J242">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K242" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>0</v>
+      </c>
+      <c r="B243" s="4">
+        <v>45382</v>
+      </c>
+      <c r="C243">
+        <v>4</v>
+      </c>
+      <c r="D243">
+        <v>122</v>
+      </c>
+      <c r="E243" s="3">
+        <v>339039990100</v>
+      </c>
+      <c r="F243" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="G243" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="H243" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="I243" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J243" s="1" cm="1">
+        <f t="array" ref="J243">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K243" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>0</v>
+      </c>
+      <c r="B244" s="4">
+        <v>45382</v>
+      </c>
+      <c r="C244">
+        <v>4</v>
+      </c>
+      <c r="D244">
+        <v>122</v>
+      </c>
+      <c r="E244" s="3">
+        <v>339039400000</v>
+      </c>
+      <c r="F244" s="2">
+        <v>22.43</v>
+      </c>
+      <c r="G244" s="2">
+        <v>77.66</v>
+      </c>
+      <c r="H244" s="2">
+        <v>131.6</v>
+      </c>
+      <c r="I244" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J244" s="1" cm="1">
+        <f t="array" ref="J244">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K244" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>0</v>
+      </c>
+      <c r="B245" s="4">
+        <v>45382</v>
+      </c>
+      <c r="C245">
+        <v>4</v>
+      </c>
+      <c r="D245">
+        <v>122</v>
+      </c>
+      <c r="E245" s="3">
+        <v>339046010100</v>
+      </c>
+      <c r="F245" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="G245" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="H245" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="I245" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J245" s="1" cm="1">
+        <f t="array" ref="J245">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K245" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>0</v>
+      </c>
+      <c r="B246" s="4">
+        <v>45382</v>
+      </c>
+      <c r="C246">
+        <v>4</v>
+      </c>
+      <c r="D246">
+        <v>122</v>
+      </c>
+      <c r="E246" s="3">
+        <v>339047000000</v>
+      </c>
+      <c r="F246" s="2">
+        <v>0</v>
+      </c>
+      <c r="G246" s="2">
+        <v>0</v>
+      </c>
+      <c r="H246" s="2">
+        <v>0</v>
+      </c>
+      <c r="I246" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J246" s="1" cm="1">
+        <f t="array" ref="J246">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K246" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>0</v>
+      </c>
+      <c r="B247" s="4">
+        <v>45382</v>
+      </c>
+      <c r="C247">
+        <v>4</v>
+      </c>
+      <c r="D247">
+        <v>122</v>
+      </c>
+      <c r="E247" s="3">
+        <v>339049010000</v>
+      </c>
+      <c r="F247" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="G247" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="H247" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="I247" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J247" s="1" cm="1">
+        <f t="array" ref="J247">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K247" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>0</v>
+      </c>
+      <c r="B248" s="4">
+        <v>45382</v>
+      </c>
+      <c r="C248">
+        <v>4</v>
+      </c>
+      <c r="D248">
+        <v>122</v>
+      </c>
+      <c r="E248" s="3">
+        <v>449052000000</v>
+      </c>
+      <c r="F248" s="2">
+        <v>0</v>
+      </c>
+      <c r="G248" s="2">
+        <v>0</v>
+      </c>
+      <c r="H248" s="2">
+        <v>0</v>
+      </c>
+      <c r="I248" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J248" s="1" cm="1">
+        <f t="array" ref="J248">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K248" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>0</v>
+      </c>
+      <c r="B249" s="4">
+        <v>45382</v>
+      </c>
+      <c r="C249">
+        <v>10</v>
+      </c>
+      <c r="D249">
+        <v>302</v>
+      </c>
+      <c r="E249" s="3">
+        <v>334041390500</v>
+      </c>
+      <c r="F249" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="G249" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="H249" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="I249" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J249" s="1" cm="1">
+        <f t="array" ref="J249">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K249" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>0</v>
+      </c>
+      <c r="B250" s="4">
+        <v>45382</v>
+      </c>
+      <c r="C250">
+        <v>10</v>
+      </c>
+      <c r="D250">
+        <v>302</v>
+      </c>
+      <c r="E250" s="3">
+        <v>334041391100</v>
+      </c>
+      <c r="F250" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="G250" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="H250" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="I250" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J250" s="1" cm="1">
+        <f t="array" ref="J250">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K250" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>0</v>
+      </c>
+      <c r="B251" s="4">
+        <v>45382</v>
+      </c>
+      <c r="C251">
+        <v>10</v>
+      </c>
+      <c r="D251">
+        <v>302</v>
+      </c>
+      <c r="E251" s="3">
+        <v>334041391000</v>
+      </c>
+      <c r="F251" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="G251" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="H251" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="I251" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J251" s="1" cm="1">
+        <f t="array" ref="J251">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K251" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualziada planilha dos consórcios
</commit_message>
<xml_diff>
--- a/auxiliar/consorcios.xlsx
+++ b/auxiliar/consorcios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everton\Desktop\Sistemas\rptgen\auxiliar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1415BC83-6DCB-447D-9064-36E52169E863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2F0773-5DC6-4C1B-A71E-0BA17974F17D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A96AC45E-B2A2-4150-B6D9-2DAA0E895429}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="13">
   <si>
     <t>COFRON</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>mes</t>
+  </si>
+  <si>
+    <t>CISA</t>
   </si>
 </sst>
 </file>
@@ -663,7 +666,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF54E884-AE1C-4BA9-AAE0-247962D6BA1D}" name="ConsorcioDespesas" displayName="ConsorcioDespesas" ref="A1:K251" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF54E884-AE1C-4BA9-AAE0-247962D6BA1D}" name="ConsorcioDespesas" displayName="ConsorcioDespesas" ref="A1:K284" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{0E4E83A9-3008-4F12-867F-9127FDCBEBC7}" name="consorcio"/>
     <tableColumn id="2" xr3:uid="{AB479D49-5AA3-4445-8011-E951C1F88768}" name="data_base"/>
@@ -1007,10 +1010,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:K251"/>
+  <dimension ref="A1:K284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
-      <selection activeCell="A205" sqref="A205"/>
+    <sheetView tabSelected="1" topLeftCell="A249" workbookViewId="0">
+      <selection activeCell="G282" sqref="G282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10558,6 +10561,1254 @@
         <v>3</v>
       </c>
     </row>
+    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>0</v>
+      </c>
+      <c r="B252" s="4">
+        <v>45412</v>
+      </c>
+      <c r="C252">
+        <v>4</v>
+      </c>
+      <c r="D252">
+        <v>122</v>
+      </c>
+      <c r="E252" s="3">
+        <v>319011010100</v>
+      </c>
+      <c r="F252" s="2">
+        <v>895.44</v>
+      </c>
+      <c r="G252" s="2">
+        <v>895.44</v>
+      </c>
+      <c r="H252" s="2">
+        <v>895.44</v>
+      </c>
+      <c r="I252" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J252" s="1" cm="1">
+        <f t="array" ref="J252">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K252" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>0</v>
+      </c>
+      <c r="B253" s="4">
+        <v>45412</v>
+      </c>
+      <c r="C253">
+        <v>4</v>
+      </c>
+      <c r="D253">
+        <v>122</v>
+      </c>
+      <c r="E253" s="3">
+        <v>319013010100</v>
+      </c>
+      <c r="F253" s="2">
+        <v>71.64</v>
+      </c>
+      <c r="G253" s="2">
+        <v>71.64</v>
+      </c>
+      <c r="H253" s="2">
+        <v>71.64</v>
+      </c>
+      <c r="I253" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J253" s="1" cm="1">
+        <f t="array" ref="J253">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K253" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>0</v>
+      </c>
+      <c r="B254" s="4">
+        <v>45412</v>
+      </c>
+      <c r="C254">
+        <v>4</v>
+      </c>
+      <c r="D254">
+        <v>122</v>
+      </c>
+      <c r="E254" s="3">
+        <v>319013020100</v>
+      </c>
+      <c r="F254" s="2">
+        <v>188.04</v>
+      </c>
+      <c r="G254" s="2">
+        <v>188.04</v>
+      </c>
+      <c r="H254" s="2">
+        <v>188.04</v>
+      </c>
+      <c r="I254" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J254" s="1" cm="1">
+        <f t="array" ref="J254">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K254" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>0</v>
+      </c>
+      <c r="B255" s="4">
+        <v>45412</v>
+      </c>
+      <c r="C255">
+        <v>4</v>
+      </c>
+      <c r="D255">
+        <v>122</v>
+      </c>
+      <c r="E255" s="3">
+        <v>339014140000</v>
+      </c>
+      <c r="F255" s="2">
+        <v>232.09</v>
+      </c>
+      <c r="G255" s="2"/>
+      <c r="H255" s="2"/>
+      <c r="I255" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J255" s="1" cm="1">
+        <f t="array" ref="J255">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K255" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>0</v>
+      </c>
+      <c r="B256" s="4">
+        <v>45412</v>
+      </c>
+      <c r="C256">
+        <v>4</v>
+      </c>
+      <c r="D256">
+        <v>122</v>
+      </c>
+      <c r="E256" s="3">
+        <v>339030000000</v>
+      </c>
+      <c r="F256" s="2">
+        <v>6.01</v>
+      </c>
+      <c r="G256" s="2">
+        <v>6.01</v>
+      </c>
+      <c r="H256" s="2"/>
+      <c r="I256" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J256" s="1" cm="1">
+        <f t="array" ref="J256">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K256" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>0</v>
+      </c>
+      <c r="B257" s="4">
+        <v>45412</v>
+      </c>
+      <c r="C257">
+        <v>4</v>
+      </c>
+      <c r="D257">
+        <v>122</v>
+      </c>
+      <c r="E257" s="3">
+        <v>339033010000</v>
+      </c>
+      <c r="F257" s="2">
+        <v>153</v>
+      </c>
+      <c r="G257" s="2">
+        <v>153</v>
+      </c>
+      <c r="H257" s="2">
+        <v>153</v>
+      </c>
+      <c r="I257" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J257" s="1" cm="1">
+        <f t="array" ref="J257">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K257" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>0</v>
+      </c>
+      <c r="B258" s="4">
+        <v>45412</v>
+      </c>
+      <c r="C258">
+        <v>4</v>
+      </c>
+      <c r="D258">
+        <v>122</v>
+      </c>
+      <c r="E258" s="3">
+        <v>339039000000</v>
+      </c>
+      <c r="F258" s="2">
+        <v>3.46</v>
+      </c>
+      <c r="G258" s="2">
+        <v>47.7</v>
+      </c>
+      <c r="H258" s="2">
+        <v>47.52</v>
+      </c>
+      <c r="I258" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J258" s="1" cm="1">
+        <f t="array" ref="J258">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K258" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>0</v>
+      </c>
+      <c r="B259" s="4">
+        <v>45412</v>
+      </c>
+      <c r="C259">
+        <v>4</v>
+      </c>
+      <c r="D259">
+        <v>122</v>
+      </c>
+      <c r="E259" s="3">
+        <v>339039990100</v>
+      </c>
+      <c r="F259" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="G259" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="H259" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="I259" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J259" s="1" cm="1">
+        <f t="array" ref="J259">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K259" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>0</v>
+      </c>
+      <c r="B260" s="4">
+        <v>45412</v>
+      </c>
+      <c r="C260">
+        <v>4</v>
+      </c>
+      <c r="D260">
+        <v>122</v>
+      </c>
+      <c r="E260" s="3">
+        <v>339039400000</v>
+      </c>
+      <c r="F260" s="2">
+        <v>0</v>
+      </c>
+      <c r="G260" s="2">
+        <v>111.6</v>
+      </c>
+      <c r="H260" s="2">
+        <v>111.6</v>
+      </c>
+      <c r="I260" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J260" s="1" cm="1">
+        <f t="array" ref="J260">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K260" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>0</v>
+      </c>
+      <c r="B261" s="4">
+        <v>45412</v>
+      </c>
+      <c r="C261">
+        <v>4</v>
+      </c>
+      <c r="D261">
+        <v>122</v>
+      </c>
+      <c r="E261" s="3">
+        <v>339046010100</v>
+      </c>
+      <c r="F261" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="G261" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="H261" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="I261" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J261" s="1" cm="1">
+        <f t="array" ref="J261">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K261" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>0</v>
+      </c>
+      <c r="B262" s="4">
+        <v>45412</v>
+      </c>
+      <c r="C262">
+        <v>4</v>
+      </c>
+      <c r="D262">
+        <v>122</v>
+      </c>
+      <c r="E262" s="3">
+        <v>339047000000</v>
+      </c>
+      <c r="F262" s="2">
+        <v>0</v>
+      </c>
+      <c r="G262" s="2">
+        <v>0</v>
+      </c>
+      <c r="H262" s="2">
+        <v>0</v>
+      </c>
+      <c r="I262" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J262" s="1" cm="1">
+        <f t="array" ref="J262">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K262" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>0</v>
+      </c>
+      <c r="B263" s="4">
+        <v>45412</v>
+      </c>
+      <c r="C263">
+        <v>4</v>
+      </c>
+      <c r="D263">
+        <v>122</v>
+      </c>
+      <c r="E263" s="3">
+        <v>339049010000</v>
+      </c>
+      <c r="F263" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="G263" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="H263" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="I263" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J263" s="1" cm="1">
+        <f t="array" ref="J263">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K263" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>0</v>
+      </c>
+      <c r="B264" s="4">
+        <v>45412</v>
+      </c>
+      <c r="C264">
+        <v>4</v>
+      </c>
+      <c r="D264">
+        <v>122</v>
+      </c>
+      <c r="E264" s="3">
+        <v>449052000000</v>
+      </c>
+      <c r="F264" s="2">
+        <v>0</v>
+      </c>
+      <c r="G264" s="2">
+        <v>0</v>
+      </c>
+      <c r="H264" s="2">
+        <v>0</v>
+      </c>
+      <c r="I264" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J264" s="1" cm="1">
+        <f t="array" ref="J264">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K264" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>0</v>
+      </c>
+      <c r="B265" s="4">
+        <v>45412</v>
+      </c>
+      <c r="C265">
+        <v>10</v>
+      </c>
+      <c r="D265">
+        <v>302</v>
+      </c>
+      <c r="E265" s="3">
+        <v>334041390500</v>
+      </c>
+      <c r="F265" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="G265" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="H265" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="I265" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J265" s="1" cm="1">
+        <f t="array" ref="J265">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K265" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>0</v>
+      </c>
+      <c r="B266" s="4">
+        <v>45412</v>
+      </c>
+      <c r="C266">
+        <v>10</v>
+      </c>
+      <c r="D266">
+        <v>302</v>
+      </c>
+      <c r="E266" s="3">
+        <v>334041391100</v>
+      </c>
+      <c r="F266" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="G266" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="H266" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="I266" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J266" s="1" cm="1">
+        <f t="array" ref="J266">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K266" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>0</v>
+      </c>
+      <c r="B267" s="4">
+        <v>45412</v>
+      </c>
+      <c r="C267">
+        <v>10</v>
+      </c>
+      <c r="D267">
+        <v>302</v>
+      </c>
+      <c r="E267" s="3">
+        <v>334041391000</v>
+      </c>
+      <c r="F267" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="G267" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="H267" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="I267" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J267" s="1" cm="1">
+        <f t="array" ref="J267">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K267" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>12</v>
+      </c>
+      <c r="B268" s="4">
+        <v>45412</v>
+      </c>
+      <c r="C268">
+        <v>10</v>
+      </c>
+      <c r="D268">
+        <v>122</v>
+      </c>
+      <c r="E268" s="3">
+        <v>319011010100</v>
+      </c>
+      <c r="F268" s="2">
+        <v>1276.03</v>
+      </c>
+      <c r="G268" s="2">
+        <v>1276.03</v>
+      </c>
+      <c r="H268" s="2">
+        <v>1276.03</v>
+      </c>
+      <c r="I268" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J268" s="1" cm="1">
+        <f t="array" ref="J268">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>2</v>
+      </c>
+      <c r="K268" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>0</v>
+      </c>
+      <c r="B269" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C269">
+        <v>4</v>
+      </c>
+      <c r="D269">
+        <v>122</v>
+      </c>
+      <c r="E269" s="3">
+        <v>319011010100</v>
+      </c>
+      <c r="F269" s="2">
+        <v>895.44</v>
+      </c>
+      <c r="G269" s="2">
+        <v>895.44</v>
+      </c>
+      <c r="H269" s="2">
+        <v>895.44</v>
+      </c>
+      <c r="I269" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J269" s="1" cm="1">
+        <f t="array" ref="J269">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K269" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>0</v>
+      </c>
+      <c r="B270" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C270">
+        <v>4</v>
+      </c>
+      <c r="D270">
+        <v>122</v>
+      </c>
+      <c r="E270" s="3">
+        <v>319013010100</v>
+      </c>
+      <c r="F270" s="2">
+        <v>71.64</v>
+      </c>
+      <c r="G270" s="2">
+        <v>71.64</v>
+      </c>
+      <c r="H270" s="2">
+        <v>71.64</v>
+      </c>
+      <c r="I270" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J270" s="1" cm="1">
+        <f t="array" ref="J270">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K270" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>0</v>
+      </c>
+      <c r="B271" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C271">
+        <v>4</v>
+      </c>
+      <c r="D271">
+        <v>122</v>
+      </c>
+      <c r="E271" s="3">
+        <v>319013020100</v>
+      </c>
+      <c r="F271" s="2">
+        <v>188.04</v>
+      </c>
+      <c r="G271" s="2">
+        <v>188.04</v>
+      </c>
+      <c r="H271" s="2">
+        <v>188.04</v>
+      </c>
+      <c r="I271" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J271" s="1" cm="1">
+        <f t="array" ref="J271">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K271" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>0</v>
+      </c>
+      <c r="B272" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C272">
+        <v>4</v>
+      </c>
+      <c r="D272">
+        <v>122</v>
+      </c>
+      <c r="E272" s="3">
+        <v>339014140000</v>
+      </c>
+      <c r="F272" s="2">
+        <v>0</v>
+      </c>
+      <c r="G272" s="2">
+        <v>232.09</v>
+      </c>
+      <c r="H272" s="2">
+        <v>232.09</v>
+      </c>
+      <c r="I272" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J272" s="1" cm="1">
+        <f t="array" ref="J272">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K272" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>0</v>
+      </c>
+      <c r="B273" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C273">
+        <v>4</v>
+      </c>
+      <c r="D273">
+        <v>122</v>
+      </c>
+      <c r="E273" s="3">
+        <v>339030000000</v>
+      </c>
+      <c r="F273" s="2">
+        <v>43.64</v>
+      </c>
+      <c r="G273" s="2">
+        <v>43.64</v>
+      </c>
+      <c r="H273" s="2">
+        <v>49.65</v>
+      </c>
+      <c r="I273" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J273" s="1" cm="1">
+        <f t="array" ref="J273">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K273" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>0</v>
+      </c>
+      <c r="B274" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C274">
+        <v>4</v>
+      </c>
+      <c r="D274">
+        <v>122</v>
+      </c>
+      <c r="E274" s="3">
+        <v>339033010000</v>
+      </c>
+      <c r="F274" s="2">
+        <v>0</v>
+      </c>
+      <c r="G274" s="2">
+        <v>0</v>
+      </c>
+      <c r="H274" s="2">
+        <v>0</v>
+      </c>
+      <c r="I274" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J274" s="1" cm="1">
+        <f t="array" ref="J274">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K274" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>0</v>
+      </c>
+      <c r="B275" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C275">
+        <v>4</v>
+      </c>
+      <c r="D275">
+        <v>122</v>
+      </c>
+      <c r="E275" s="3">
+        <v>339039000000</v>
+      </c>
+      <c r="F275" s="2">
+        <v>135.08000000000001</v>
+      </c>
+      <c r="G275" s="2">
+        <v>54.2</v>
+      </c>
+      <c r="H275" s="2">
+        <v>64.150000000000006</v>
+      </c>
+      <c r="I275" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J275" s="1" cm="1">
+        <f t="array" ref="J275">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K275" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>0</v>
+      </c>
+      <c r="B276" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C276">
+        <v>4</v>
+      </c>
+      <c r="D276">
+        <v>122</v>
+      </c>
+      <c r="E276" s="3">
+        <v>339039990100</v>
+      </c>
+      <c r="F276" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="G276" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="H276" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="I276" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J276" s="1" cm="1">
+        <f t="array" ref="J276">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K276" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>0</v>
+      </c>
+      <c r="B277" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C277">
+        <v>4</v>
+      </c>
+      <c r="D277">
+        <v>122</v>
+      </c>
+      <c r="E277" s="3">
+        <v>339039400000</v>
+      </c>
+      <c r="F277" s="2">
+        <v>-366.33</v>
+      </c>
+      <c r="G277" s="2">
+        <v>171.98</v>
+      </c>
+      <c r="H277" s="2">
+        <v>115.61</v>
+      </c>
+      <c r="I277" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J277" s="1" cm="1">
+        <f t="array" ref="J277">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K277" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>0</v>
+      </c>
+      <c r="B278" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C278">
+        <v>4</v>
+      </c>
+      <c r="D278">
+        <v>122</v>
+      </c>
+      <c r="E278" s="3">
+        <v>339046010100</v>
+      </c>
+      <c r="F278" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="G278" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="H278" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="I278" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J278" s="1" cm="1">
+        <f t="array" ref="J278">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K278" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>0</v>
+      </c>
+      <c r="B279" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C279">
+        <v>4</v>
+      </c>
+      <c r="D279">
+        <v>122</v>
+      </c>
+      <c r="E279" s="3">
+        <v>339047000000</v>
+      </c>
+      <c r="F279" s="2">
+        <v>0</v>
+      </c>
+      <c r="G279" s="2">
+        <v>0</v>
+      </c>
+      <c r="H279" s="2">
+        <v>0</v>
+      </c>
+      <c r="I279" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J279" s="1" cm="1">
+        <f t="array" ref="J279">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K279" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>0</v>
+      </c>
+      <c r="B280" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C280">
+        <v>4</v>
+      </c>
+      <c r="D280">
+        <v>122</v>
+      </c>
+      <c r="E280" s="3">
+        <v>339049010000</v>
+      </c>
+      <c r="F280" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="G280" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="H280" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="I280" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J280" s="1" cm="1">
+        <f t="array" ref="J280">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K280" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>0</v>
+      </c>
+      <c r="B281" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C281">
+        <v>4</v>
+      </c>
+      <c r="D281">
+        <v>122</v>
+      </c>
+      <c r="E281" s="3">
+        <v>449052000000</v>
+      </c>
+      <c r="F281" s="2">
+        <v>0</v>
+      </c>
+      <c r="G281" s="2">
+        <v>0</v>
+      </c>
+      <c r="H281" s="2">
+        <v>0</v>
+      </c>
+      <c r="I281" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J281" s="1" cm="1">
+        <f t="array" ref="J281">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K281" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>0</v>
+      </c>
+      <c r="B282" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C282">
+        <v>10</v>
+      </c>
+      <c r="D282">
+        <v>302</v>
+      </c>
+      <c r="E282" s="3">
+        <v>334041390500</v>
+      </c>
+      <c r="F282" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="G282" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="H282" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="I282" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J282" s="1" cm="1">
+        <f t="array" ref="J282">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K282" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>0</v>
+      </c>
+      <c r="B283" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C283">
+        <v>10</v>
+      </c>
+      <c r="D283">
+        <v>302</v>
+      </c>
+      <c r="E283" s="3">
+        <v>334041391100</v>
+      </c>
+      <c r="F283" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="G283" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="H283" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="I283" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J283" s="1" cm="1">
+        <f t="array" ref="J283">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K283" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>0</v>
+      </c>
+      <c r="B284" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C284">
+        <v>10</v>
+      </c>
+      <c r="D284">
+        <v>302</v>
+      </c>
+      <c r="E284" s="3">
+        <v>334041391000</v>
+      </c>
+      <c r="F284" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="G284" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="H284" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="I284" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J284" s="1" cm="1">
+        <f t="array" ref="J284">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K284" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adicionado dados de consoriocs
</commit_message>
<xml_diff>
--- a/auxiliar/consorcios.xlsx
+++ b/auxiliar/consorcios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everton\Desktop\Sistemas\rptgen\auxiliar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2F0773-5DC6-4C1B-A71E-0BA17974F17D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6231BD10-E48C-46E2-817E-C78C2789B2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A96AC45E-B2A2-4150-B6D9-2DAA0E895429}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="13">
   <si>
     <t>COFRON</t>
   </si>
@@ -666,7 +666,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF54E884-AE1C-4BA9-AAE0-247962D6BA1D}" name="ConsorcioDespesas" displayName="ConsorcioDespesas" ref="A1:K284" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF54E884-AE1C-4BA9-AAE0-247962D6BA1D}" name="ConsorcioDespesas" displayName="ConsorcioDespesas" ref="A1:K300" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{0E4E83A9-3008-4F12-867F-9127FDCBEBC7}" name="consorcio"/>
     <tableColumn id="2" xr3:uid="{AB479D49-5AA3-4445-8011-E951C1F88768}" name="data_base"/>
@@ -1010,10 +1010,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:K284"/>
+  <dimension ref="A1:K300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A249" workbookViewId="0">
-      <selection activeCell="G282" sqref="G282"/>
+    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="G298" sqref="G298:H300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11809,6 +11809,614 @@
         <v>5</v>
       </c>
     </row>
+    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>0</v>
+      </c>
+      <c r="B285" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C285">
+        <v>4</v>
+      </c>
+      <c r="D285">
+        <v>122</v>
+      </c>
+      <c r="E285" s="3">
+        <v>319011010100</v>
+      </c>
+      <c r="F285" s="2">
+        <v>1343.17</v>
+      </c>
+      <c r="G285" s="2">
+        <v>1343.17</v>
+      </c>
+      <c r="H285" s="2">
+        <v>1343.17</v>
+      </c>
+      <c r="I285" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J285" s="1" cm="1">
+        <f t="array" ref="J285">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K285" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>0</v>
+      </c>
+      <c r="B286" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C286">
+        <v>4</v>
+      </c>
+      <c r="D286">
+        <v>122</v>
+      </c>
+      <c r="E286" s="3">
+        <v>319013010100</v>
+      </c>
+      <c r="F286" s="2">
+        <v>71.64</v>
+      </c>
+      <c r="G286" s="2">
+        <v>71.64</v>
+      </c>
+      <c r="H286" s="2">
+        <v>71.64</v>
+      </c>
+      <c r="I286" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J286" s="1" cm="1">
+        <f t="array" ref="J286">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K286" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>0</v>
+      </c>
+      <c r="B287" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C287">
+        <v>4</v>
+      </c>
+      <c r="D287">
+        <v>122</v>
+      </c>
+      <c r="E287" s="3">
+        <v>319013020100</v>
+      </c>
+      <c r="F287" s="2">
+        <v>188.04</v>
+      </c>
+      <c r="G287" s="2">
+        <v>188.04</v>
+      </c>
+      <c r="H287" s="2">
+        <v>188.04</v>
+      </c>
+      <c r="I287" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J287" s="1" cm="1">
+        <f t="array" ref="J287">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K287" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>0</v>
+      </c>
+      <c r="B288" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C288">
+        <v>4</v>
+      </c>
+      <c r="D288">
+        <v>122</v>
+      </c>
+      <c r="E288" s="3">
+        <v>339014140000</v>
+      </c>
+      <c r="F288" s="2">
+        <v>53.65</v>
+      </c>
+      <c r="G288" s="2">
+        <v>53.65</v>
+      </c>
+      <c r="H288" s="2">
+        <v>53.65</v>
+      </c>
+      <c r="I288" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J288" s="1" cm="1">
+        <f t="array" ref="J288">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K288" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>0</v>
+      </c>
+      <c r="B289" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C289">
+        <v>4</v>
+      </c>
+      <c r="D289">
+        <v>122</v>
+      </c>
+      <c r="E289" s="3">
+        <v>339030000000</v>
+      </c>
+      <c r="F289" s="2">
+        <v>0</v>
+      </c>
+      <c r="G289" s="2">
+        <v>0</v>
+      </c>
+      <c r="H289" s="2">
+        <v>0</v>
+      </c>
+      <c r="I289" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J289" s="1" cm="1">
+        <f t="array" ref="J289">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K289" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>0</v>
+      </c>
+      <c r="B290" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C290">
+        <v>4</v>
+      </c>
+      <c r="D290">
+        <v>122</v>
+      </c>
+      <c r="E290" s="3">
+        <v>339033010000</v>
+      </c>
+      <c r="F290" s="2">
+        <v>11.98</v>
+      </c>
+      <c r="G290" s="2">
+        <v>11.98</v>
+      </c>
+      <c r="H290" s="2">
+        <v>11.98</v>
+      </c>
+      <c r="I290" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J290" s="1" cm="1">
+        <f t="array" ref="J290">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K290" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>0</v>
+      </c>
+      <c r="B291" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C291">
+        <v>4</v>
+      </c>
+      <c r="D291">
+        <v>122</v>
+      </c>
+      <c r="E291" s="3">
+        <v>339039000000</v>
+      </c>
+      <c r="F291" s="2">
+        <v>3.46</v>
+      </c>
+      <c r="G291" s="2">
+        <v>54.33</v>
+      </c>
+      <c r="H291" s="2">
+        <v>54.2</v>
+      </c>
+      <c r="I291" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J291" s="1" cm="1">
+        <f t="array" ref="J291">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K291" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>0</v>
+      </c>
+      <c r="B292" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C292">
+        <v>4</v>
+      </c>
+      <c r="D292">
+        <v>122</v>
+      </c>
+      <c r="E292" s="3">
+        <v>339039990100</v>
+      </c>
+      <c r="F292" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="G292" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="H292" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="I292" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J292" s="1" cm="1">
+        <f t="array" ref="J292">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K292" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>0</v>
+      </c>
+      <c r="B293" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C293">
+        <v>4</v>
+      </c>
+      <c r="D293">
+        <v>122</v>
+      </c>
+      <c r="E293" s="3">
+        <v>339039400000</v>
+      </c>
+      <c r="F293" s="2">
+        <v>56.37</v>
+      </c>
+      <c r="G293" s="2">
+        <v>111.6</v>
+      </c>
+      <c r="H293" s="2">
+        <v>111.6</v>
+      </c>
+      <c r="I293" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J293" s="1" cm="1">
+        <f t="array" ref="J293">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K293" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>0</v>
+      </c>
+      <c r="B294" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C294">
+        <v>4</v>
+      </c>
+      <c r="D294">
+        <v>122</v>
+      </c>
+      <c r="E294" s="3">
+        <v>339046010100</v>
+      </c>
+      <c r="F294" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="G294" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="H294" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="I294" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J294" s="1" cm="1">
+        <f t="array" ref="J294">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K294" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>0</v>
+      </c>
+      <c r="B295" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C295">
+        <v>4</v>
+      </c>
+      <c r="D295">
+        <v>122</v>
+      </c>
+      <c r="E295" s="3">
+        <v>339047000000</v>
+      </c>
+      <c r="F295" s="2">
+        <v>9.1</v>
+      </c>
+      <c r="G295" s="2">
+        <v>9.1</v>
+      </c>
+      <c r="H295" s="2">
+        <v>9.1</v>
+      </c>
+      <c r="I295" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J295" s="1" cm="1">
+        <f t="array" ref="J295">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K295" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>0</v>
+      </c>
+      <c r="B296" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C296">
+        <v>4</v>
+      </c>
+      <c r="D296">
+        <v>122</v>
+      </c>
+      <c r="E296" s="3">
+        <v>339049010000</v>
+      </c>
+      <c r="F296" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="G296" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="H296" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="I296" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J296" s="1" cm="1">
+        <f t="array" ref="J296">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K296" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>0</v>
+      </c>
+      <c r="B297" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C297">
+        <v>4</v>
+      </c>
+      <c r="D297">
+        <v>122</v>
+      </c>
+      <c r="E297" s="3">
+        <v>449052000000</v>
+      </c>
+      <c r="F297" s="2">
+        <v>0</v>
+      </c>
+      <c r="G297" s="2">
+        <v>0</v>
+      </c>
+      <c r="H297" s="2">
+        <v>0</v>
+      </c>
+      <c r="I297" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J297" s="1" cm="1">
+        <f t="array" ref="J297">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K297" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>0</v>
+      </c>
+      <c r="B298" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C298">
+        <v>10</v>
+      </c>
+      <c r="D298">
+        <v>302</v>
+      </c>
+      <c r="E298" s="3">
+        <v>334041390500</v>
+      </c>
+      <c r="F298" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="G298" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="H298" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="I298" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J298" s="1" cm="1">
+        <f t="array" ref="J298">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K298" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>0</v>
+      </c>
+      <c r="B299" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C299">
+        <v>10</v>
+      </c>
+      <c r="D299">
+        <v>302</v>
+      </c>
+      <c r="E299" s="3">
+        <v>334041391100</v>
+      </c>
+      <c r="F299" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="G299" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="H299" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="I299" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J299" s="1" cm="1">
+        <f t="array" ref="J299">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K299" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>0</v>
+      </c>
+      <c r="B300" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C300">
+        <v>10</v>
+      </c>
+      <c r="D300">
+        <v>302</v>
+      </c>
+      <c r="E300" s="3">
+        <v>334041391000</v>
+      </c>
+      <c r="F300" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="G300" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="H300" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="I300" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J300" s="1" cm="1">
+        <f t="array" ref="J300">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K300" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix: correção no cálculo da DTP do executivo
</commit_message>
<xml_diff>
--- a/auxiliar/consorcios.xlsx
+++ b/auxiliar/consorcios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everton\Desktop\Sistemas\rptgen\auxiliar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6231BD10-E48C-46E2-817E-C78C2789B2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D9031C-6809-4CCD-A494-29C7AD5AFD7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A96AC45E-B2A2-4150-B6D9-2DAA0E895429}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="13">
   <si>
     <t>COFRON</t>
   </si>
@@ -666,7 +666,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF54E884-AE1C-4BA9-AAE0-247962D6BA1D}" name="ConsorcioDespesas" displayName="ConsorcioDespesas" ref="A1:K300" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF54E884-AE1C-4BA9-AAE0-247962D6BA1D}" name="ConsorcioDespesas" displayName="ConsorcioDespesas" ref="A1:K284" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{0E4E83A9-3008-4F12-867F-9127FDCBEBC7}" name="consorcio"/>
     <tableColumn id="2" xr3:uid="{AB479D49-5AA3-4445-8011-E951C1F88768}" name="data_base"/>
@@ -1010,10 +1010,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:K300"/>
+  <dimension ref="A1:K284"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
-      <selection activeCell="G298" sqref="G298:H300"/>
+      <selection activeCell="A285" sqref="A285:XFD300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11809,614 +11809,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A285" t="s">
-        <v>0</v>
-      </c>
-      <c r="B285" s="4">
-        <v>45473</v>
-      </c>
-      <c r="C285">
-        <v>4</v>
-      </c>
-      <c r="D285">
-        <v>122</v>
-      </c>
-      <c r="E285" s="3">
-        <v>319011010100</v>
-      </c>
-      <c r="F285" s="2">
-        <v>1343.17</v>
-      </c>
-      <c r="G285" s="2">
-        <v>1343.17</v>
-      </c>
-      <c r="H285" s="2">
-        <v>1343.17</v>
-      </c>
-      <c r="I285" s="1">
-        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>2024</v>
-      </c>
-      <c r="J285" s="1" cm="1">
-        <f t="array" ref="J285">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
-        <v>3</v>
-      </c>
-      <c r="K285" s="1">
-        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A286" t="s">
-        <v>0</v>
-      </c>
-      <c r="B286" s="4">
-        <v>45473</v>
-      </c>
-      <c r="C286">
-        <v>4</v>
-      </c>
-      <c r="D286">
-        <v>122</v>
-      </c>
-      <c r="E286" s="3">
-        <v>319013010100</v>
-      </c>
-      <c r="F286" s="2">
-        <v>71.64</v>
-      </c>
-      <c r="G286" s="2">
-        <v>71.64</v>
-      </c>
-      <c r="H286" s="2">
-        <v>71.64</v>
-      </c>
-      <c r="I286" s="1">
-        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>2024</v>
-      </c>
-      <c r="J286" s="1" cm="1">
-        <f t="array" ref="J286">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
-        <v>3</v>
-      </c>
-      <c r="K286" s="1">
-        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A287" t="s">
-        <v>0</v>
-      </c>
-      <c r="B287" s="4">
-        <v>45473</v>
-      </c>
-      <c r="C287">
-        <v>4</v>
-      </c>
-      <c r="D287">
-        <v>122</v>
-      </c>
-      <c r="E287" s="3">
-        <v>319013020100</v>
-      </c>
-      <c r="F287" s="2">
-        <v>188.04</v>
-      </c>
-      <c r="G287" s="2">
-        <v>188.04</v>
-      </c>
-      <c r="H287" s="2">
-        <v>188.04</v>
-      </c>
-      <c r="I287" s="1">
-        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>2024</v>
-      </c>
-      <c r="J287" s="1" cm="1">
-        <f t="array" ref="J287">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
-        <v>3</v>
-      </c>
-      <c r="K287" s="1">
-        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A288" t="s">
-        <v>0</v>
-      </c>
-      <c r="B288" s="4">
-        <v>45473</v>
-      </c>
-      <c r="C288">
-        <v>4</v>
-      </c>
-      <c r="D288">
-        <v>122</v>
-      </c>
-      <c r="E288" s="3">
-        <v>339014140000</v>
-      </c>
-      <c r="F288" s="2">
-        <v>53.65</v>
-      </c>
-      <c r="G288" s="2">
-        <v>53.65</v>
-      </c>
-      <c r="H288" s="2">
-        <v>53.65</v>
-      </c>
-      <c r="I288" s="1">
-        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>2024</v>
-      </c>
-      <c r="J288" s="1" cm="1">
-        <f t="array" ref="J288">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
-        <v>3</v>
-      </c>
-      <c r="K288" s="1">
-        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A289" t="s">
-        <v>0</v>
-      </c>
-      <c r="B289" s="4">
-        <v>45473</v>
-      </c>
-      <c r="C289">
-        <v>4</v>
-      </c>
-      <c r="D289">
-        <v>122</v>
-      </c>
-      <c r="E289" s="3">
-        <v>339030000000</v>
-      </c>
-      <c r="F289" s="2">
-        <v>0</v>
-      </c>
-      <c r="G289" s="2">
-        <v>0</v>
-      </c>
-      <c r="H289" s="2">
-        <v>0</v>
-      </c>
-      <c r="I289" s="1">
-        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>2024</v>
-      </c>
-      <c r="J289" s="1" cm="1">
-        <f t="array" ref="J289">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
-        <v>3</v>
-      </c>
-      <c r="K289" s="1">
-        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A290" t="s">
-        <v>0</v>
-      </c>
-      <c r="B290" s="4">
-        <v>45473</v>
-      </c>
-      <c r="C290">
-        <v>4</v>
-      </c>
-      <c r="D290">
-        <v>122</v>
-      </c>
-      <c r="E290" s="3">
-        <v>339033010000</v>
-      </c>
-      <c r="F290" s="2">
-        <v>11.98</v>
-      </c>
-      <c r="G290" s="2">
-        <v>11.98</v>
-      </c>
-      <c r="H290" s="2">
-        <v>11.98</v>
-      </c>
-      <c r="I290" s="1">
-        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>2024</v>
-      </c>
-      <c r="J290" s="1" cm="1">
-        <f t="array" ref="J290">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
-        <v>3</v>
-      </c>
-      <c r="K290" s="1">
-        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A291" t="s">
-        <v>0</v>
-      </c>
-      <c r="B291" s="4">
-        <v>45473</v>
-      </c>
-      <c r="C291">
-        <v>4</v>
-      </c>
-      <c r="D291">
-        <v>122</v>
-      </c>
-      <c r="E291" s="3">
-        <v>339039000000</v>
-      </c>
-      <c r="F291" s="2">
-        <v>3.46</v>
-      </c>
-      <c r="G291" s="2">
-        <v>54.33</v>
-      </c>
-      <c r="H291" s="2">
-        <v>54.2</v>
-      </c>
-      <c r="I291" s="1">
-        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>2024</v>
-      </c>
-      <c r="J291" s="1" cm="1">
-        <f t="array" ref="J291">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
-        <v>3</v>
-      </c>
-      <c r="K291" s="1">
-        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A292" t="s">
-        <v>0</v>
-      </c>
-      <c r="B292" s="4">
-        <v>45473</v>
-      </c>
-      <c r="C292">
-        <v>4</v>
-      </c>
-      <c r="D292">
-        <v>122</v>
-      </c>
-      <c r="E292" s="3">
-        <v>339039990100</v>
-      </c>
-      <c r="F292" s="2">
-        <v>59.11</v>
-      </c>
-      <c r="G292" s="2">
-        <v>59.11</v>
-      </c>
-      <c r="H292" s="2">
-        <v>59.11</v>
-      </c>
-      <c r="I292" s="1">
-        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>2024</v>
-      </c>
-      <c r="J292" s="1" cm="1">
-        <f t="array" ref="J292">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
-        <v>3</v>
-      </c>
-      <c r="K292" s="1">
-        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A293" t="s">
-        <v>0</v>
-      </c>
-      <c r="B293" s="4">
-        <v>45473</v>
-      </c>
-      <c r="C293">
-        <v>4</v>
-      </c>
-      <c r="D293">
-        <v>122</v>
-      </c>
-      <c r="E293" s="3">
-        <v>339039400000</v>
-      </c>
-      <c r="F293" s="2">
-        <v>56.37</v>
-      </c>
-      <c r="G293" s="2">
-        <v>111.6</v>
-      </c>
-      <c r="H293" s="2">
-        <v>111.6</v>
-      </c>
-      <c r="I293" s="1">
-        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>2024</v>
-      </c>
-      <c r="J293" s="1" cm="1">
-        <f t="array" ref="J293">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
-        <v>3</v>
-      </c>
-      <c r="K293" s="1">
-        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A294" t="s">
-        <v>0</v>
-      </c>
-      <c r="B294" s="4">
-        <v>45473</v>
-      </c>
-      <c r="C294">
-        <v>4</v>
-      </c>
-      <c r="D294">
-        <v>122</v>
-      </c>
-      <c r="E294" s="3">
-        <v>339046010100</v>
-      </c>
-      <c r="F294" s="2">
-        <v>53.48</v>
-      </c>
-      <c r="G294" s="2">
-        <v>53.48</v>
-      </c>
-      <c r="H294" s="2">
-        <v>53.48</v>
-      </c>
-      <c r="I294" s="1">
-        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>2024</v>
-      </c>
-      <c r="J294" s="1" cm="1">
-        <f t="array" ref="J294">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
-        <v>3</v>
-      </c>
-      <c r="K294" s="1">
-        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A295" t="s">
-        <v>0</v>
-      </c>
-      <c r="B295" s="4">
-        <v>45473</v>
-      </c>
-      <c r="C295">
-        <v>4</v>
-      </c>
-      <c r="D295">
-        <v>122</v>
-      </c>
-      <c r="E295" s="3">
-        <v>339047000000</v>
-      </c>
-      <c r="F295" s="2">
-        <v>9.1</v>
-      </c>
-      <c r="G295" s="2">
-        <v>9.1</v>
-      </c>
-      <c r="H295" s="2">
-        <v>9.1</v>
-      </c>
-      <c r="I295" s="1">
-        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>2024</v>
-      </c>
-      <c r="J295" s="1" cm="1">
-        <f t="array" ref="J295">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
-        <v>3</v>
-      </c>
-      <c r="K295" s="1">
-        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A296" t="s">
-        <v>0</v>
-      </c>
-      <c r="B296" s="4">
-        <v>45473</v>
-      </c>
-      <c r="C296">
-        <v>4</v>
-      </c>
-      <c r="D296">
-        <v>122</v>
-      </c>
-      <c r="E296" s="3">
-        <v>339049010000</v>
-      </c>
-      <c r="F296" s="2">
-        <v>1.96</v>
-      </c>
-      <c r="G296" s="2">
-        <v>1.96</v>
-      </c>
-      <c r="H296" s="2">
-        <v>1.96</v>
-      </c>
-      <c r="I296" s="1">
-        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>2024</v>
-      </c>
-      <c r="J296" s="1" cm="1">
-        <f t="array" ref="J296">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
-        <v>3</v>
-      </c>
-      <c r="K296" s="1">
-        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A297" t="s">
-        <v>0</v>
-      </c>
-      <c r="B297" s="4">
-        <v>45473</v>
-      </c>
-      <c r="C297">
-        <v>4</v>
-      </c>
-      <c r="D297">
-        <v>122</v>
-      </c>
-      <c r="E297" s="3">
-        <v>449052000000</v>
-      </c>
-      <c r="F297" s="2">
-        <v>0</v>
-      </c>
-      <c r="G297" s="2">
-        <v>0</v>
-      </c>
-      <c r="H297" s="2">
-        <v>0</v>
-      </c>
-      <c r="I297" s="1">
-        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>2024</v>
-      </c>
-      <c r="J297" s="1" cm="1">
-        <f t="array" ref="J297">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
-        <v>3</v>
-      </c>
-      <c r="K297" s="1">
-        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A298" t="s">
-        <v>0</v>
-      </c>
-      <c r="B298" s="4">
-        <v>45473</v>
-      </c>
-      <c r="C298">
-        <v>10</v>
-      </c>
-      <c r="D298">
-        <v>302</v>
-      </c>
-      <c r="E298" s="3">
-        <v>334041390500</v>
-      </c>
-      <c r="F298" s="2">
-        <v>9273.68</v>
-      </c>
-      <c r="G298" s="2">
-        <v>9273.68</v>
-      </c>
-      <c r="H298" s="2">
-        <v>9273.68</v>
-      </c>
-      <c r="I298" s="1">
-        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>2024</v>
-      </c>
-      <c r="J298" s="1" cm="1">
-        <f t="array" ref="J298">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
-        <v>3</v>
-      </c>
-      <c r="K298" s="1">
-        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A299" t="s">
-        <v>0</v>
-      </c>
-      <c r="B299" s="4">
-        <v>45473</v>
-      </c>
-      <c r="C299">
-        <v>10</v>
-      </c>
-      <c r="D299">
-        <v>302</v>
-      </c>
-      <c r="E299" s="3">
-        <v>334041391100</v>
-      </c>
-      <c r="F299" s="2">
-        <v>865.54</v>
-      </c>
-      <c r="G299" s="2">
-        <v>865.54</v>
-      </c>
-      <c r="H299" s="2">
-        <v>865.54</v>
-      </c>
-      <c r="I299" s="1">
-        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>2024</v>
-      </c>
-      <c r="J299" s="1" cm="1">
-        <f t="array" ref="J299">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
-        <v>3</v>
-      </c>
-      <c r="K299" s="1">
-        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A300" t="s">
-        <v>0</v>
-      </c>
-      <c r="B300" s="4">
-        <v>45473</v>
-      </c>
-      <c r="C300">
-        <v>10</v>
-      </c>
-      <c r="D300">
-        <v>302</v>
-      </c>
-      <c r="E300" s="3">
-        <v>334041391000</v>
-      </c>
-      <c r="F300" s="2">
-        <v>655.91</v>
-      </c>
-      <c r="G300" s="2">
-        <v>655.91</v>
-      </c>
-      <c r="H300" s="2">
-        <v>655.91</v>
-      </c>
-      <c r="I300" s="1">
-        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>2024</v>
-      </c>
-      <c r="J300" s="1" cm="1">
-        <f t="array" ref="J300">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
-        <v>3</v>
-      </c>
-      <c r="K300" s="1">
-        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix: ajustado BF para a IPC 06 revisada em junho de 2024
</commit_message>
<xml_diff>
--- a/auxiliar/consorcios.xlsx
+++ b/auxiliar/consorcios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everton\Desktop\Sistemas\rptgen\auxiliar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6231BD10-E48C-46E2-817E-C78C2789B2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6841ED74-35CB-4A5C-ABFC-86A8DB435B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A96AC45E-B2A2-4150-B6D9-2DAA0E895429}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="13">
   <si>
     <t>COFRON</t>
   </si>
@@ -666,7 +666,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF54E884-AE1C-4BA9-AAE0-247962D6BA1D}" name="ConsorcioDespesas" displayName="ConsorcioDespesas" ref="A1:K300" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF54E884-AE1C-4BA9-AAE0-247962D6BA1D}" name="ConsorcioDespesas" displayName="ConsorcioDespesas" ref="A1:K301" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{0E4E83A9-3008-4F12-867F-9127FDCBEBC7}" name="consorcio"/>
     <tableColumn id="2" xr3:uid="{AB479D49-5AA3-4445-8011-E951C1F88768}" name="data_base"/>
@@ -1010,10 +1010,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:K300"/>
+  <dimension ref="A1:K301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
-      <selection activeCell="G298" sqref="G298:H300"/>
+    <sheetView tabSelected="1" topLeftCell="A266" workbookViewId="0">
+      <selection activeCell="F302" sqref="F302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12417,6 +12417,44 @@
         <v>6</v>
       </c>
     </row>
+    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>12</v>
+      </c>
+      <c r="B301" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C301">
+        <v>10</v>
+      </c>
+      <c r="D301">
+        <v>122</v>
+      </c>
+      <c r="E301" s="3">
+        <v>319011010100</v>
+      </c>
+      <c r="F301" s="2">
+        <v>1279.78</v>
+      </c>
+      <c r="G301" s="2">
+        <v>1279.78</v>
+      </c>
+      <c r="H301" s="2">
+        <v>1279.78</v>
+      </c>
+      <c r="I301" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J301" s="1" cm="1">
+        <f t="array" ref="J301">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>3</v>
+      </c>
+      <c r="K301" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: Implementado cálculo das dotações de folha e vale.
</commit_message>
<xml_diff>
--- a/auxiliar/consorcios.xlsx
+++ b/auxiliar/consorcios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everton\Desktop\Sistemas\rptgen\auxiliar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6841ED74-35CB-4A5C-ABFC-86A8DB435B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023A58C0-037F-483B-A2DA-B39F8E1E8055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A96AC45E-B2A2-4150-B6D9-2DAA0E895429}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="13">
   <si>
     <t>COFRON</t>
   </si>
@@ -666,7 +666,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF54E884-AE1C-4BA9-AAE0-247962D6BA1D}" name="ConsorcioDespesas" displayName="ConsorcioDespesas" ref="A1:K301" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF54E884-AE1C-4BA9-AAE0-247962D6BA1D}" name="ConsorcioDespesas" displayName="ConsorcioDespesas" ref="A1:K317" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{0E4E83A9-3008-4F12-867F-9127FDCBEBC7}" name="consorcio"/>
     <tableColumn id="2" xr3:uid="{AB479D49-5AA3-4445-8011-E951C1F88768}" name="data_base"/>
@@ -1010,10 +1010,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:K301"/>
+  <dimension ref="A1:K317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A266" workbookViewId="0">
-      <selection activeCell="F302" sqref="F302"/>
+    <sheetView tabSelected="1" topLeftCell="A282" workbookViewId="0">
+      <selection activeCell="H314" sqref="H314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12455,6 +12455,614 @@
         <v>6</v>
       </c>
     </row>
+    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>0</v>
+      </c>
+      <c r="B302" s="4">
+        <v>45504</v>
+      </c>
+      <c r="C302">
+        <v>4</v>
+      </c>
+      <c r="D302">
+        <v>122</v>
+      </c>
+      <c r="E302" s="3">
+        <v>319011010100</v>
+      </c>
+      <c r="F302" s="2">
+        <v>895.44</v>
+      </c>
+      <c r="G302" s="2">
+        <v>895.44</v>
+      </c>
+      <c r="H302" s="2">
+        <v>895.44</v>
+      </c>
+      <c r="I302" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J302" s="1" cm="1">
+        <f t="array" ref="J302">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K302" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>0</v>
+      </c>
+      <c r="B303" s="4">
+        <v>45504</v>
+      </c>
+      <c r="C303">
+        <v>4</v>
+      </c>
+      <c r="D303">
+        <v>122</v>
+      </c>
+      <c r="E303" s="3">
+        <v>319013010100</v>
+      </c>
+      <c r="F303" s="2">
+        <v>107.45</v>
+      </c>
+      <c r="G303" s="2">
+        <v>107.45</v>
+      </c>
+      <c r="H303" s="2">
+        <v>107.45</v>
+      </c>
+      <c r="I303" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J303" s="1" cm="1">
+        <f t="array" ref="J303">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K303" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>0</v>
+      </c>
+      <c r="B304" s="4">
+        <v>45504</v>
+      </c>
+      <c r="C304">
+        <v>4</v>
+      </c>
+      <c r="D304">
+        <v>122</v>
+      </c>
+      <c r="E304" s="3">
+        <v>319013020100</v>
+      </c>
+      <c r="F304" s="2">
+        <v>188.04</v>
+      </c>
+      <c r="G304" s="2">
+        <v>188.04</v>
+      </c>
+      <c r="H304" s="2">
+        <v>188.04</v>
+      </c>
+      <c r="I304" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J304" s="1" cm="1">
+        <f t="array" ref="J304">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K304" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>0</v>
+      </c>
+      <c r="B305" s="4">
+        <v>45504</v>
+      </c>
+      <c r="C305">
+        <v>4</v>
+      </c>
+      <c r="D305">
+        <v>122</v>
+      </c>
+      <c r="E305" s="3">
+        <v>339014140000</v>
+      </c>
+      <c r="F305" s="2">
+        <v>0</v>
+      </c>
+      <c r="G305" s="2">
+        <v>0</v>
+      </c>
+      <c r="H305" s="2">
+        <v>0</v>
+      </c>
+      <c r="I305" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J305" s="1" cm="1">
+        <f t="array" ref="J305">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K305" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>0</v>
+      </c>
+      <c r="B306" s="4">
+        <v>45504</v>
+      </c>
+      <c r="C306">
+        <v>4</v>
+      </c>
+      <c r="D306">
+        <v>122</v>
+      </c>
+      <c r="E306" s="3">
+        <v>339030000000</v>
+      </c>
+      <c r="F306" s="2">
+        <v>89.3</v>
+      </c>
+      <c r="G306" s="2">
+        <v>89.3</v>
+      </c>
+      <c r="H306" s="2">
+        <v>89.3</v>
+      </c>
+      <c r="I306" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J306" s="1" cm="1">
+        <f t="array" ref="J306">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K306" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>0</v>
+      </c>
+      <c r="B307" s="4">
+        <v>45504</v>
+      </c>
+      <c r="C307">
+        <v>4</v>
+      </c>
+      <c r="D307">
+        <v>122</v>
+      </c>
+      <c r="E307" s="3">
+        <v>339033010000</v>
+      </c>
+      <c r="F307" s="2">
+        <v>0</v>
+      </c>
+      <c r="G307" s="2">
+        <v>0</v>
+      </c>
+      <c r="H307" s="2">
+        <v>0</v>
+      </c>
+      <c r="I307" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J307" s="1" cm="1">
+        <f t="array" ref="J307">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K307" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>0</v>
+      </c>
+      <c r="B308" s="4">
+        <v>45504</v>
+      </c>
+      <c r="C308">
+        <v>4</v>
+      </c>
+      <c r="D308">
+        <v>122</v>
+      </c>
+      <c r="E308" s="3">
+        <v>339039000000</v>
+      </c>
+      <c r="F308" s="2">
+        <v>67.89</v>
+      </c>
+      <c r="G308" s="2">
+        <v>121.46</v>
+      </c>
+      <c r="H308" s="2">
+        <v>59.79</v>
+      </c>
+      <c r="I308" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J308" s="1" cm="1">
+        <f t="array" ref="J308">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K308" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>0</v>
+      </c>
+      <c r="B309" s="4">
+        <v>45504</v>
+      </c>
+      <c r="C309">
+        <v>4</v>
+      </c>
+      <c r="D309">
+        <v>122</v>
+      </c>
+      <c r="E309" s="3">
+        <v>339039990100</v>
+      </c>
+      <c r="F309" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="G309" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="H309" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="I309" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J309" s="1" cm="1">
+        <f t="array" ref="J309">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K309" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>0</v>
+      </c>
+      <c r="B310" s="4">
+        <v>45504</v>
+      </c>
+      <c r="C310">
+        <v>4</v>
+      </c>
+      <c r="D310">
+        <v>122</v>
+      </c>
+      <c r="E310" s="3">
+        <v>339039400000</v>
+      </c>
+      <c r="F310" s="2">
+        <v>79.290000000000006</v>
+      </c>
+      <c r="G310" s="2">
+        <v>134.52000000000001</v>
+      </c>
+      <c r="H310" s="2">
+        <v>134.53</v>
+      </c>
+      <c r="I310" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J310" s="1" cm="1">
+        <f t="array" ref="J310">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K310" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>0</v>
+      </c>
+      <c r="B311" s="4">
+        <v>45504</v>
+      </c>
+      <c r="C311">
+        <v>4</v>
+      </c>
+      <c r="D311">
+        <v>122</v>
+      </c>
+      <c r="E311" s="3">
+        <v>339046010100</v>
+      </c>
+      <c r="F311" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="G311" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="H311" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="I311" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J311" s="1" cm="1">
+        <f t="array" ref="J311">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K311" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>0</v>
+      </c>
+      <c r="B312" s="4">
+        <v>45504</v>
+      </c>
+      <c r="C312">
+        <v>4</v>
+      </c>
+      <c r="D312">
+        <v>122</v>
+      </c>
+      <c r="E312" s="3">
+        <v>339047000000</v>
+      </c>
+      <c r="F312" s="2">
+        <v>0</v>
+      </c>
+      <c r="G312" s="2">
+        <v>0</v>
+      </c>
+      <c r="H312" s="2">
+        <v>0</v>
+      </c>
+      <c r="I312" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J312" s="1" cm="1">
+        <f t="array" ref="J312">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K312" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>0</v>
+      </c>
+      <c r="B313" s="4">
+        <v>45504</v>
+      </c>
+      <c r="C313">
+        <v>4</v>
+      </c>
+      <c r="D313">
+        <v>122</v>
+      </c>
+      <c r="E313" s="3">
+        <v>339049010000</v>
+      </c>
+      <c r="F313" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="G313" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="H313" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="I313" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J313" s="1" cm="1">
+        <f t="array" ref="J313">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K313" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>0</v>
+      </c>
+      <c r="B314" s="4">
+        <v>45504</v>
+      </c>
+      <c r="C314">
+        <v>4</v>
+      </c>
+      <c r="D314">
+        <v>122</v>
+      </c>
+      <c r="E314" s="3">
+        <v>449052000000</v>
+      </c>
+      <c r="F314" s="2">
+        <v>0</v>
+      </c>
+      <c r="G314" s="2">
+        <v>0</v>
+      </c>
+      <c r="H314" s="2">
+        <v>0</v>
+      </c>
+      <c r="I314" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J314" s="1" cm="1">
+        <f t="array" ref="J314">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K314" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>0</v>
+      </c>
+      <c r="B315" s="4">
+        <v>45504</v>
+      </c>
+      <c r="C315">
+        <v>10</v>
+      </c>
+      <c r="D315">
+        <v>302</v>
+      </c>
+      <c r="E315" s="3">
+        <v>334041390500</v>
+      </c>
+      <c r="F315" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="G315" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="H315" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="I315" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J315" s="1" cm="1">
+        <f t="array" ref="J315">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K315" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>0</v>
+      </c>
+      <c r="B316" s="4">
+        <v>45504</v>
+      </c>
+      <c r="C316">
+        <v>10</v>
+      </c>
+      <c r="D316">
+        <v>302</v>
+      </c>
+      <c r="E316" s="3">
+        <v>334041391100</v>
+      </c>
+      <c r="F316" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="G316" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="H316" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="I316" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J316" s="1" cm="1">
+        <f t="array" ref="J316">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K316" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>0</v>
+      </c>
+      <c r="B317" s="4">
+        <v>45504</v>
+      </c>
+      <c r="C317">
+        <v>10</v>
+      </c>
+      <c r="D317">
+        <v>302</v>
+      </c>
+      <c r="E317" s="3">
+        <v>334041391000</v>
+      </c>
+      <c r="F317" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="G317" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="H317" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="I317" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J317" s="1" cm="1">
+        <f t="array" ref="J317">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K317" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix: Exclusão de planilhas não utilizadas na geração de índice de pessoal
A planilha do RREO A14 Competo stava com nomes errados.
</commit_message>
<xml_diff>
--- a/auxiliar/consorcios.xlsx
+++ b/auxiliar/consorcios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everton\Desktop\Sistemas\rptgen\auxiliar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023A58C0-037F-483B-A2DA-B39F8E1E8055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3431F6-EB40-4ECA-A68A-A814728721BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A96AC45E-B2A2-4150-B6D9-2DAA0E895429}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="13">
   <si>
     <t>COFRON</t>
   </si>
@@ -666,7 +666,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF54E884-AE1C-4BA9-AAE0-247962D6BA1D}" name="ConsorcioDespesas" displayName="ConsorcioDespesas" ref="A1:K317" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF54E884-AE1C-4BA9-AAE0-247962D6BA1D}" name="ConsorcioDespesas" displayName="ConsorcioDespesas" ref="A1:K333" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{0E4E83A9-3008-4F12-867F-9127FDCBEBC7}" name="consorcio"/>
     <tableColumn id="2" xr3:uid="{AB479D49-5AA3-4445-8011-E951C1F88768}" name="data_base"/>
@@ -1010,10 +1010,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:K317"/>
+  <dimension ref="A1:K333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A282" workbookViewId="0">
-      <selection activeCell="H314" sqref="H314"/>
+    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
+      <selection activeCell="F319" sqref="F319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13063,6 +13063,614 @@
         <v>7</v>
       </c>
     </row>
+    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>0</v>
+      </c>
+      <c r="B318" s="4">
+        <v>45535</v>
+      </c>
+      <c r="C318">
+        <v>4</v>
+      </c>
+      <c r="D318">
+        <v>122</v>
+      </c>
+      <c r="E318" s="3">
+        <v>319011010100</v>
+      </c>
+      <c r="F318" s="2">
+        <v>1201.8499999999999</v>
+      </c>
+      <c r="G318" s="2">
+        <v>1201.8499999999999</v>
+      </c>
+      <c r="H318" s="2">
+        <v>1201.8499999999999</v>
+      </c>
+      <c r="I318" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J318" s="1" cm="1">
+        <f t="array" ref="J318">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K318" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>0</v>
+      </c>
+      <c r="B319" s="4">
+        <v>45535</v>
+      </c>
+      <c r="C319">
+        <v>4</v>
+      </c>
+      <c r="D319">
+        <v>122</v>
+      </c>
+      <c r="E319" s="3">
+        <v>319013010100</v>
+      </c>
+      <c r="F319" s="2">
+        <v>79.81</v>
+      </c>
+      <c r="G319" s="2">
+        <v>79.81</v>
+      </c>
+      <c r="H319" s="2">
+        <v>71.64</v>
+      </c>
+      <c r="I319" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J319" s="1" cm="1">
+        <f t="array" ref="J319">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K319" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="320" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>0</v>
+      </c>
+      <c r="B320" s="4">
+        <v>45535</v>
+      </c>
+      <c r="C320">
+        <v>4</v>
+      </c>
+      <c r="D320">
+        <v>122</v>
+      </c>
+      <c r="E320" s="3">
+        <v>319013020100</v>
+      </c>
+      <c r="F320" s="2">
+        <v>209.49</v>
+      </c>
+      <c r="G320" s="2">
+        <v>209.49</v>
+      </c>
+      <c r="H320" s="2">
+        <v>188.04</v>
+      </c>
+      <c r="I320" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J320" s="1" cm="1">
+        <f t="array" ref="J320">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K320" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>0</v>
+      </c>
+      <c r="B321" s="4">
+        <v>45535</v>
+      </c>
+      <c r="C321">
+        <v>4</v>
+      </c>
+      <c r="D321">
+        <v>122</v>
+      </c>
+      <c r="E321" s="3">
+        <v>339014140000</v>
+      </c>
+      <c r="F321" s="2">
+        <v>0</v>
+      </c>
+      <c r="G321" s="2">
+        <v>0</v>
+      </c>
+      <c r="H321" s="2">
+        <v>0</v>
+      </c>
+      <c r="I321" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J321" s="1" cm="1">
+        <f t="array" ref="J321">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K321" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>0</v>
+      </c>
+      <c r="B322" s="4">
+        <v>45535</v>
+      </c>
+      <c r="C322">
+        <v>4</v>
+      </c>
+      <c r="D322">
+        <v>122</v>
+      </c>
+      <c r="E322" s="3">
+        <v>339030000000</v>
+      </c>
+      <c r="F322" s="2">
+        <v>0</v>
+      </c>
+      <c r="G322" s="2">
+        <v>0</v>
+      </c>
+      <c r="H322" s="2">
+        <v>0</v>
+      </c>
+      <c r="I322" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J322" s="1" cm="1">
+        <f t="array" ref="J322">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K322" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>0</v>
+      </c>
+      <c r="B323" s="4">
+        <v>45535</v>
+      </c>
+      <c r="C323">
+        <v>4</v>
+      </c>
+      <c r="D323">
+        <v>122</v>
+      </c>
+      <c r="E323" s="3">
+        <v>339033010000</v>
+      </c>
+      <c r="F323" s="2">
+        <v>0</v>
+      </c>
+      <c r="G323" s="2">
+        <v>0</v>
+      </c>
+      <c r="H323" s="2">
+        <v>0</v>
+      </c>
+      <c r="I323" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J323" s="1" cm="1">
+        <f t="array" ref="J323">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K323" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>0</v>
+      </c>
+      <c r="B324" s="4">
+        <v>45535</v>
+      </c>
+      <c r="C324">
+        <v>4</v>
+      </c>
+      <c r="D324">
+        <v>122</v>
+      </c>
+      <c r="E324" s="3">
+        <v>339039000000</v>
+      </c>
+      <c r="F324" s="2">
+        <v>3.46</v>
+      </c>
+      <c r="G324" s="2">
+        <v>59.3</v>
+      </c>
+      <c r="H324" s="2">
+        <v>119.64</v>
+      </c>
+      <c r="I324" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J324" s="1" cm="1">
+        <f t="array" ref="J324">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K324" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>0</v>
+      </c>
+      <c r="B325" s="4">
+        <v>45535</v>
+      </c>
+      <c r="C325">
+        <v>4</v>
+      </c>
+      <c r="D325">
+        <v>122</v>
+      </c>
+      <c r="E325" s="3">
+        <v>339039990100</v>
+      </c>
+      <c r="F325" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="G325" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="H325" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="I325" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J325" s="1" cm="1">
+        <f t="array" ref="J325">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K325" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>0</v>
+      </c>
+      <c r="B326" s="4">
+        <v>45535</v>
+      </c>
+      <c r="C326">
+        <v>4</v>
+      </c>
+      <c r="D326">
+        <v>122</v>
+      </c>
+      <c r="E326" s="3">
+        <v>339039400000</v>
+      </c>
+      <c r="F326" s="2">
+        <v>56.37</v>
+      </c>
+      <c r="G326" s="2">
+        <v>111.6</v>
+      </c>
+      <c r="H326" s="2">
+        <v>111.58</v>
+      </c>
+      <c r="I326" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J326" s="1" cm="1">
+        <f t="array" ref="J326">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K326" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="327" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>0</v>
+      </c>
+      <c r="B327" s="4">
+        <v>45535</v>
+      </c>
+      <c r="C327">
+        <v>4</v>
+      </c>
+      <c r="D327">
+        <v>122</v>
+      </c>
+      <c r="E327" s="3">
+        <v>339046010100</v>
+      </c>
+      <c r="F327" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="G327" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="H327" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="I327" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J327" s="1" cm="1">
+        <f t="array" ref="J327">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K327" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>0</v>
+      </c>
+      <c r="B328" s="4">
+        <v>45535</v>
+      </c>
+      <c r="C328">
+        <v>4</v>
+      </c>
+      <c r="D328">
+        <v>122</v>
+      </c>
+      <c r="E328" s="3">
+        <v>339047000000</v>
+      </c>
+      <c r="F328" s="2">
+        <v>0</v>
+      </c>
+      <c r="G328" s="2">
+        <v>0</v>
+      </c>
+      <c r="H328" s="2">
+        <v>0</v>
+      </c>
+      <c r="I328" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J328" s="1" cm="1">
+        <f t="array" ref="J328">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K328" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>0</v>
+      </c>
+      <c r="B329" s="4">
+        <v>45535</v>
+      </c>
+      <c r="C329">
+        <v>4</v>
+      </c>
+      <c r="D329">
+        <v>122</v>
+      </c>
+      <c r="E329" s="3">
+        <v>339049010000</v>
+      </c>
+      <c r="F329" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="G329" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="H329" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="I329" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J329" s="1" cm="1">
+        <f t="array" ref="J329">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K329" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="330" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>0</v>
+      </c>
+      <c r="B330" s="4">
+        <v>45535</v>
+      </c>
+      <c r="C330">
+        <v>4</v>
+      </c>
+      <c r="D330">
+        <v>122</v>
+      </c>
+      <c r="E330" s="3">
+        <v>449052000000</v>
+      </c>
+      <c r="F330" s="2">
+        <v>116.48</v>
+      </c>
+      <c r="G330" s="2">
+        <v>116.48</v>
+      </c>
+      <c r="H330" s="2">
+        <v>116.48</v>
+      </c>
+      <c r="I330" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J330" s="1" cm="1">
+        <f t="array" ref="J330">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K330" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="331" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>0</v>
+      </c>
+      <c r="B331" s="4">
+        <v>45535</v>
+      </c>
+      <c r="C331">
+        <v>10</v>
+      </c>
+      <c r="D331">
+        <v>302</v>
+      </c>
+      <c r="E331" s="3">
+        <v>334041390500</v>
+      </c>
+      <c r="F331" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="G331" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="H331" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="I331" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J331" s="1" cm="1">
+        <f t="array" ref="J331">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K331" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="332" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>0</v>
+      </c>
+      <c r="B332" s="4">
+        <v>45535</v>
+      </c>
+      <c r="C332">
+        <v>10</v>
+      </c>
+      <c r="D332">
+        <v>302</v>
+      </c>
+      <c r="E332" s="3">
+        <v>334041391100</v>
+      </c>
+      <c r="F332" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="G332" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="H332" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="I332" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J332" s="1" cm="1">
+        <f t="array" ref="J332">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K332" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="333" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>0</v>
+      </c>
+      <c r="B333" s="4">
+        <v>45535</v>
+      </c>
+      <c r="C333">
+        <v>10</v>
+      </c>
+      <c r="D333">
+        <v>302</v>
+      </c>
+      <c r="E333" s="3">
+        <v>334041391000</v>
+      </c>
+      <c r="F333" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="G333" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="H333" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="I333" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J333" s="1" cm="1">
+        <f t="array" ref="J333">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>4</v>
+      </c>
+      <c r="K333" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix: Corrigido bug no balanço financeiro.
</commit_message>
<xml_diff>
--- a/auxiliar/consorcios.xlsx
+++ b/auxiliar/consorcios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everton\Desktop\Sistemas\rptgen\auxiliar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFC05DD-E45F-41A4-A08F-67CBBAD55548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7EE26B-2B13-4CBA-8ED3-07A0BD336957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A96AC45E-B2A2-4150-B6D9-2DAA0E895429}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="13">
   <si>
     <t>COFRON</t>
   </si>
@@ -666,7 +666,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF54E884-AE1C-4BA9-AAE0-247962D6BA1D}" name="ConsorcioDespesas" displayName="ConsorcioDespesas" ref="A1:K349" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF54E884-AE1C-4BA9-AAE0-247962D6BA1D}" name="ConsorcioDespesas" displayName="ConsorcioDespesas" ref="A1:K365" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{0E4E83A9-3008-4F12-867F-9127FDCBEBC7}" name="consorcio"/>
     <tableColumn id="2" xr3:uid="{AB479D49-5AA3-4445-8011-E951C1F88768}" name="data_base"/>
@@ -1010,10 +1010,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:K349"/>
+  <dimension ref="A1:K365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A311" workbookViewId="0">
-      <selection activeCell="F350" sqref="F350"/>
+    <sheetView tabSelected="1" topLeftCell="A330" workbookViewId="0">
+      <selection activeCell="H366" sqref="H366"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14279,6 +14279,614 @@
         <v>9</v>
       </c>
     </row>
+    <row r="350" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>0</v>
+      </c>
+      <c r="B350" s="4">
+        <v>45596</v>
+      </c>
+      <c r="C350">
+        <v>4</v>
+      </c>
+      <c r="D350">
+        <v>122</v>
+      </c>
+      <c r="E350" s="3">
+        <v>319011010100</v>
+      </c>
+      <c r="F350" s="2">
+        <v>900.4</v>
+      </c>
+      <c r="G350" s="2">
+        <v>900.4</v>
+      </c>
+      <c r="H350" s="2">
+        <v>900.4</v>
+      </c>
+      <c r="I350" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J350" s="1" cm="1">
+        <f t="array" ref="J350">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>5</v>
+      </c>
+      <c r="K350" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="351" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>0</v>
+      </c>
+      <c r="B351" s="4">
+        <v>45596</v>
+      </c>
+      <c r="C351">
+        <v>4</v>
+      </c>
+      <c r="D351">
+        <v>122</v>
+      </c>
+      <c r="E351" s="3">
+        <v>319013010100</v>
+      </c>
+      <c r="F351" s="2">
+        <v>72.03</v>
+      </c>
+      <c r="G351" s="2">
+        <v>72.03</v>
+      </c>
+      <c r="H351" s="2">
+        <v>73.540000000000006</v>
+      </c>
+      <c r="I351" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J351" s="1" cm="1">
+        <f t="array" ref="J351">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>5</v>
+      </c>
+      <c r="K351" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="352" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>0</v>
+      </c>
+      <c r="B352" s="4">
+        <v>45596</v>
+      </c>
+      <c r="C352">
+        <v>4</v>
+      </c>
+      <c r="D352">
+        <v>122</v>
+      </c>
+      <c r="E352" s="3">
+        <v>319013020100</v>
+      </c>
+      <c r="F352" s="2">
+        <v>189.08</v>
+      </c>
+      <c r="G352" s="2">
+        <v>189.08</v>
+      </c>
+      <c r="H352" s="2">
+        <v>193.04</v>
+      </c>
+      <c r="I352" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J352" s="1" cm="1">
+        <f t="array" ref="J352">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>5</v>
+      </c>
+      <c r="K352" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="353" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>0</v>
+      </c>
+      <c r="B353" s="4">
+        <v>45596</v>
+      </c>
+      <c r="C353">
+        <v>4</v>
+      </c>
+      <c r="D353">
+        <v>122</v>
+      </c>
+      <c r="E353" s="3">
+        <v>339014140000</v>
+      </c>
+      <c r="F353" s="2">
+        <v>0</v>
+      </c>
+      <c r="G353" s="2">
+        <v>0</v>
+      </c>
+      <c r="H353" s="2">
+        <v>0</v>
+      </c>
+      <c r="I353" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J353" s="1" cm="1">
+        <f t="array" ref="J353">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>5</v>
+      </c>
+      <c r="K353" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="354" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>0</v>
+      </c>
+      <c r="B354" s="4">
+        <v>45596</v>
+      </c>
+      <c r="C354">
+        <v>4</v>
+      </c>
+      <c r="D354">
+        <v>122</v>
+      </c>
+      <c r="E354" s="3">
+        <v>339030000000</v>
+      </c>
+      <c r="F354" s="2">
+        <v>0</v>
+      </c>
+      <c r="G354" s="2">
+        <v>15.51</v>
+      </c>
+      <c r="H354" s="2">
+        <v>15.51</v>
+      </c>
+      <c r="I354" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J354" s="1" cm="1">
+        <f t="array" ref="J354">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>5</v>
+      </c>
+      <c r="K354" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="355" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>0</v>
+      </c>
+      <c r="B355" s="4">
+        <v>45596</v>
+      </c>
+      <c r="C355">
+        <v>4</v>
+      </c>
+      <c r="D355">
+        <v>122</v>
+      </c>
+      <c r="E355" s="3">
+        <v>339033010000</v>
+      </c>
+      <c r="F355" s="2">
+        <v>0</v>
+      </c>
+      <c r="G355" s="2">
+        <v>0</v>
+      </c>
+      <c r="H355" s="2">
+        <v>0</v>
+      </c>
+      <c r="I355" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J355" s="1" cm="1">
+        <f t="array" ref="J355">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>5</v>
+      </c>
+      <c r="K355" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="356" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>0</v>
+      </c>
+      <c r="B356" s="4">
+        <v>45596</v>
+      </c>
+      <c r="C356">
+        <v>4</v>
+      </c>
+      <c r="D356">
+        <v>122</v>
+      </c>
+      <c r="E356" s="3">
+        <v>339039000000</v>
+      </c>
+      <c r="F356" s="2">
+        <v>47.29</v>
+      </c>
+      <c r="G356" s="2">
+        <v>61.04</v>
+      </c>
+      <c r="H356" s="2">
+        <v>50.26</v>
+      </c>
+      <c r="I356" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J356" s="1" cm="1">
+        <f t="array" ref="J356">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>5</v>
+      </c>
+      <c r="K356" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="357" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>0</v>
+      </c>
+      <c r="B357" s="4">
+        <v>45596</v>
+      </c>
+      <c r="C357">
+        <v>4</v>
+      </c>
+      <c r="D357">
+        <v>122</v>
+      </c>
+      <c r="E357" s="3">
+        <v>339039990100</v>
+      </c>
+      <c r="F357" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="G357" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="H357" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="I357" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J357" s="1" cm="1">
+        <f t="array" ref="J357">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>5</v>
+      </c>
+      <c r="K357" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="358" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>0</v>
+      </c>
+      <c r="B358" s="4">
+        <v>45596</v>
+      </c>
+      <c r="C358">
+        <v>4</v>
+      </c>
+      <c r="D358">
+        <v>122</v>
+      </c>
+      <c r="E358" s="3">
+        <v>339039400000</v>
+      </c>
+      <c r="F358" s="2">
+        <v>0</v>
+      </c>
+      <c r="G358" s="2">
+        <v>111.6</v>
+      </c>
+      <c r="H358" s="2">
+        <v>111.6</v>
+      </c>
+      <c r="I358" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J358" s="1" cm="1">
+        <f t="array" ref="J358">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>5</v>
+      </c>
+      <c r="K358" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="359" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>0</v>
+      </c>
+      <c r="B359" s="4">
+        <v>45596</v>
+      </c>
+      <c r="C359">
+        <v>4</v>
+      </c>
+      <c r="D359">
+        <v>122</v>
+      </c>
+      <c r="E359" s="3">
+        <v>339046010100</v>
+      </c>
+      <c r="F359" s="2">
+        <v>53.66</v>
+      </c>
+      <c r="G359" s="2">
+        <v>53.66</v>
+      </c>
+      <c r="H359" s="2">
+        <v>53.66</v>
+      </c>
+      <c r="I359" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J359" s="1" cm="1">
+        <f t="array" ref="J359">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>5</v>
+      </c>
+      <c r="K359" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="360" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>0</v>
+      </c>
+      <c r="B360" s="4">
+        <v>45596</v>
+      </c>
+      <c r="C360">
+        <v>4</v>
+      </c>
+      <c r="D360">
+        <v>122</v>
+      </c>
+      <c r="E360" s="3">
+        <v>339047000000</v>
+      </c>
+      <c r="F360" s="2">
+        <v>0</v>
+      </c>
+      <c r="G360" s="2">
+        <v>0</v>
+      </c>
+      <c r="H360" s="2">
+        <v>0</v>
+      </c>
+      <c r="I360" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J360" s="1" cm="1">
+        <f t="array" ref="J360">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>5</v>
+      </c>
+      <c r="K360" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="361" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>0</v>
+      </c>
+      <c r="B361" s="4">
+        <v>45596</v>
+      </c>
+      <c r="C361">
+        <v>4</v>
+      </c>
+      <c r="D361">
+        <v>122</v>
+      </c>
+      <c r="E361" s="3">
+        <v>339049010000</v>
+      </c>
+      <c r="F361" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="G361" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="H361" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="I361" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J361" s="1" cm="1">
+        <f t="array" ref="J361">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>5</v>
+      </c>
+      <c r="K361" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="362" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>0</v>
+      </c>
+      <c r="B362" s="4">
+        <v>45596</v>
+      </c>
+      <c r="C362">
+        <v>4</v>
+      </c>
+      <c r="D362">
+        <v>122</v>
+      </c>
+      <c r="E362" s="3">
+        <v>449052000000</v>
+      </c>
+      <c r="F362" s="2">
+        <v>0</v>
+      </c>
+      <c r="G362" s="2">
+        <v>0</v>
+      </c>
+      <c r="H362" s="2">
+        <v>0</v>
+      </c>
+      <c r="I362" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J362" s="1" cm="1">
+        <f t="array" ref="J362">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>5</v>
+      </c>
+      <c r="K362" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="363" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>0</v>
+      </c>
+      <c r="B363" s="4">
+        <v>45596</v>
+      </c>
+      <c r="C363">
+        <v>10</v>
+      </c>
+      <c r="D363">
+        <v>302</v>
+      </c>
+      <c r="E363" s="3">
+        <v>334041390500</v>
+      </c>
+      <c r="F363" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="G363" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="H363" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="I363" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J363" s="1" cm="1">
+        <f t="array" ref="J363">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>5</v>
+      </c>
+      <c r="K363" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="364" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>0</v>
+      </c>
+      <c r="B364" s="4">
+        <v>45596</v>
+      </c>
+      <c r="C364">
+        <v>10</v>
+      </c>
+      <c r="D364">
+        <v>302</v>
+      </c>
+      <c r="E364" s="3">
+        <v>334041391100</v>
+      </c>
+      <c r="F364" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="G364" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="H364" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="I364" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J364" s="1" cm="1">
+        <f t="array" ref="J364">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>5</v>
+      </c>
+      <c r="K364" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="365" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>0</v>
+      </c>
+      <c r="B365" s="4">
+        <v>45596</v>
+      </c>
+      <c r="C365">
+        <v>10</v>
+      </c>
+      <c r="D365">
+        <v>302</v>
+      </c>
+      <c r="E365" s="3">
+        <v>334041391000</v>
+      </c>
+      <c r="F365" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="G365" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="H365" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="I365" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J365" s="1" cm="1">
+        <f t="array" ref="J365">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>5</v>
+      </c>
+      <c r="K365" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Despesas com consórcios updated
</commit_message>
<xml_diff>
--- a/auxiliar/consorcios.xlsx
+++ b/auxiliar/consorcios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everton\Desktop\Sistemas\rptgen\auxiliar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7EE26B-2B13-4CBA-8ED3-07A0BD336957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BBC76F-F5BA-467D-9E42-C536B962F7CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A96AC45E-B2A2-4150-B6D9-2DAA0E895429}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="13">
   <si>
     <t>COFRON</t>
   </si>
@@ -666,7 +666,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF54E884-AE1C-4BA9-AAE0-247962D6BA1D}" name="ConsorcioDespesas" displayName="ConsorcioDespesas" ref="A1:K365" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF54E884-AE1C-4BA9-AAE0-247962D6BA1D}" name="ConsorcioDespesas" displayName="ConsorcioDespesas" ref="A1:K381" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{0E4E83A9-3008-4F12-867F-9127FDCBEBC7}" name="consorcio"/>
     <tableColumn id="2" xr3:uid="{AB479D49-5AA3-4445-8011-E951C1F88768}" name="data_base"/>
@@ -1010,10 +1010,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:K365"/>
+  <dimension ref="A1:K381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A330" workbookViewId="0">
-      <selection activeCell="H366" sqref="H366"/>
+    <sheetView tabSelected="1" topLeftCell="A346" workbookViewId="0">
+      <selection activeCell="F379" sqref="F379"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14887,6 +14887,614 @@
         <v>10</v>
       </c>
     </row>
+    <row r="366" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>0</v>
+      </c>
+      <c r="B366" s="4">
+        <v>45626</v>
+      </c>
+      <c r="C366">
+        <v>4</v>
+      </c>
+      <c r="D366">
+        <v>122</v>
+      </c>
+      <c r="E366" s="3">
+        <v>319011010100</v>
+      </c>
+      <c r="F366" s="2">
+        <v>1355.05</v>
+      </c>
+      <c r="G366" s="2">
+        <v>1355.05</v>
+      </c>
+      <c r="H366" s="2">
+        <v>1355.05</v>
+      </c>
+      <c r="I366" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J366" s="1" cm="1">
+        <f t="array" ref="J366">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K366" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="367" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>0</v>
+      </c>
+      <c r="B367" s="4">
+        <v>45626</v>
+      </c>
+      <c r="C367">
+        <v>4</v>
+      </c>
+      <c r="D367">
+        <v>122</v>
+      </c>
+      <c r="E367" s="3">
+        <v>319013010100</v>
+      </c>
+      <c r="F367" s="2">
+        <v>72.11</v>
+      </c>
+      <c r="G367" s="2">
+        <v>72.11</v>
+      </c>
+      <c r="H367" s="2">
+        <v>72.03</v>
+      </c>
+      <c r="I367" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J367" s="1" cm="1">
+        <f t="array" ref="J367">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K367" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="368" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>0</v>
+      </c>
+      <c r="B368" s="4">
+        <v>45626</v>
+      </c>
+      <c r="C368">
+        <v>4</v>
+      </c>
+      <c r="D368">
+        <v>122</v>
+      </c>
+      <c r="E368" s="3">
+        <v>319013020100</v>
+      </c>
+      <c r="F368" s="2">
+        <v>189.29</v>
+      </c>
+      <c r="G368" s="2">
+        <v>189.29</v>
+      </c>
+      <c r="H368" s="2">
+        <v>189.08</v>
+      </c>
+      <c r="I368" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J368" s="1" cm="1">
+        <f t="array" ref="J368">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K368" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="369" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
+        <v>0</v>
+      </c>
+      <c r="B369" s="4">
+        <v>45626</v>
+      </c>
+      <c r="C369">
+        <v>4</v>
+      </c>
+      <c r="D369">
+        <v>122</v>
+      </c>
+      <c r="E369" s="3">
+        <v>339014140000</v>
+      </c>
+      <c r="F369" s="2">
+        <v>0</v>
+      </c>
+      <c r="G369" s="2">
+        <v>0</v>
+      </c>
+      <c r="H369" s="2">
+        <v>0</v>
+      </c>
+      <c r="I369" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J369" s="1" cm="1">
+        <f t="array" ref="J369">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K369" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="370" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
+        <v>0</v>
+      </c>
+      <c r="B370" s="4">
+        <v>45626</v>
+      </c>
+      <c r="C370">
+        <v>4</v>
+      </c>
+      <c r="D370">
+        <v>122</v>
+      </c>
+      <c r="E370" s="3">
+        <v>339030000000</v>
+      </c>
+      <c r="F370" s="2">
+        <v>64.069999999999993</v>
+      </c>
+      <c r="G370" s="2">
+        <v>64.069999999999993</v>
+      </c>
+      <c r="H370" s="2">
+        <v>64.069999999999993</v>
+      </c>
+      <c r="I370" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J370" s="1" cm="1">
+        <f t="array" ref="J370">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K370" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="371" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>0</v>
+      </c>
+      <c r="B371" s="4">
+        <v>45626</v>
+      </c>
+      <c r="C371">
+        <v>4</v>
+      </c>
+      <c r="D371">
+        <v>122</v>
+      </c>
+      <c r="E371" s="3">
+        <v>339033010000</v>
+      </c>
+      <c r="F371" s="2">
+        <v>0</v>
+      </c>
+      <c r="G371" s="2">
+        <v>0</v>
+      </c>
+      <c r="H371" s="2">
+        <v>0</v>
+      </c>
+      <c r="I371" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J371" s="1" cm="1">
+        <f t="array" ref="J371">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K371" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="372" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>0</v>
+      </c>
+      <c r="B372" s="4">
+        <v>45626</v>
+      </c>
+      <c r="C372">
+        <v>4</v>
+      </c>
+      <c r="D372">
+        <v>122</v>
+      </c>
+      <c r="E372" s="3">
+        <v>339039000000</v>
+      </c>
+      <c r="F372" s="2">
+        <v>31.47</v>
+      </c>
+      <c r="G372" s="2">
+        <v>89.63</v>
+      </c>
+      <c r="H372" s="2">
+        <v>81.8</v>
+      </c>
+      <c r="I372" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J372" s="1" cm="1">
+        <f t="array" ref="J372">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K372" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="373" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>0</v>
+      </c>
+      <c r="B373" s="4">
+        <v>45626</v>
+      </c>
+      <c r="C373">
+        <v>4</v>
+      </c>
+      <c r="D373">
+        <v>122</v>
+      </c>
+      <c r="E373" s="3">
+        <v>339039990100</v>
+      </c>
+      <c r="F373" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="G373" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="H373" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="I373" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J373" s="1" cm="1">
+        <f t="array" ref="J373">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K373" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="374" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>0</v>
+      </c>
+      <c r="B374" s="4">
+        <v>45626</v>
+      </c>
+      <c r="C374">
+        <v>4</v>
+      </c>
+      <c r="D374">
+        <v>122</v>
+      </c>
+      <c r="E374" s="3">
+        <v>339039400000</v>
+      </c>
+      <c r="F374" s="2">
+        <v>247.52</v>
+      </c>
+      <c r="G374" s="2">
+        <v>111.6</v>
+      </c>
+      <c r="H374" s="2">
+        <v>111.6</v>
+      </c>
+      <c r="I374" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J374" s="1" cm="1">
+        <f t="array" ref="J374">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K374" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="375" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>0</v>
+      </c>
+      <c r="B375" s="4">
+        <v>45626</v>
+      </c>
+      <c r="C375">
+        <v>4</v>
+      </c>
+      <c r="D375">
+        <v>122</v>
+      </c>
+      <c r="E375" s="3">
+        <v>339046010100</v>
+      </c>
+      <c r="F375" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="G375" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="H375" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="I375" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J375" s="1" cm="1">
+        <f t="array" ref="J375">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K375" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="376" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>0</v>
+      </c>
+      <c r="B376" s="4">
+        <v>45626</v>
+      </c>
+      <c r="C376">
+        <v>4</v>
+      </c>
+      <c r="D376">
+        <v>122</v>
+      </c>
+      <c r="E376" s="3">
+        <v>339047000000</v>
+      </c>
+      <c r="F376" s="2">
+        <v>0</v>
+      </c>
+      <c r="G376" s="2">
+        <v>0</v>
+      </c>
+      <c r="H376" s="2">
+        <v>0</v>
+      </c>
+      <c r="I376" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J376" s="1" cm="1">
+        <f t="array" ref="J376">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K376" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="377" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>0</v>
+      </c>
+      <c r="B377" s="4">
+        <v>45626</v>
+      </c>
+      <c r="C377">
+        <v>4</v>
+      </c>
+      <c r="D377">
+        <v>122</v>
+      </c>
+      <c r="E377" s="3">
+        <v>339049010000</v>
+      </c>
+      <c r="F377" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="G377" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="H377" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="I377" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J377" s="1" cm="1">
+        <f t="array" ref="J377">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K377" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="378" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
+        <v>0</v>
+      </c>
+      <c r="B378" s="4">
+        <v>45626</v>
+      </c>
+      <c r="C378">
+        <v>4</v>
+      </c>
+      <c r="D378">
+        <v>122</v>
+      </c>
+      <c r="E378" s="3">
+        <v>449052000000</v>
+      </c>
+      <c r="F378" s="2">
+        <v>0</v>
+      </c>
+      <c r="G378" s="2">
+        <v>0</v>
+      </c>
+      <c r="H378" s="2">
+        <v>0</v>
+      </c>
+      <c r="I378" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J378" s="1" cm="1">
+        <f t="array" ref="J378">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K378" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="379" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>0</v>
+      </c>
+      <c r="B379" s="4">
+        <v>45626</v>
+      </c>
+      <c r="C379">
+        <v>10</v>
+      </c>
+      <c r="D379">
+        <v>302</v>
+      </c>
+      <c r="E379" s="3">
+        <v>334041390500</v>
+      </c>
+      <c r="F379" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="G379" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="H379" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="I379" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J379" s="1" cm="1">
+        <f t="array" ref="J379">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K379" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="380" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>0</v>
+      </c>
+      <c r="B380" s="4">
+        <v>45626</v>
+      </c>
+      <c r="C380">
+        <v>10</v>
+      </c>
+      <c r="D380">
+        <v>302</v>
+      </c>
+      <c r="E380" s="3">
+        <v>334041391100</v>
+      </c>
+      <c r="F380" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="G380" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="H380" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="I380" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J380" s="1" cm="1">
+        <f t="array" ref="J380">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K380" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="381" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>0</v>
+      </c>
+      <c r="B381" s="4">
+        <v>45626</v>
+      </c>
+      <c r="C381">
+        <v>10</v>
+      </c>
+      <c r="D381">
+        <v>302</v>
+      </c>
+      <c r="E381" s="3">
+        <v>334041391000</v>
+      </c>
+      <c r="F381" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="G381" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="H381" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="I381" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J381" s="1" cm="1">
+        <f t="array" ref="J381">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K381" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix: DCASP fechada para a PM.
</commit_message>
<xml_diff>
--- a/auxiliar/consorcios.xlsx
+++ b/auxiliar/consorcios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everton\Desktop\Sistemas\rptgen\auxiliar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769598DB-5E4D-4883-AF8B-AAC0566BC416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE04FADA-8E28-4E26-8B24-B98FB7EB1D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A96AC45E-B2A2-4150-B6D9-2DAA0E895429}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="13">
   <si>
     <t>COFRON</t>
   </si>
@@ -666,7 +666,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF54E884-AE1C-4BA9-AAE0-247962D6BA1D}" name="ConsorcioDespesas" displayName="ConsorcioDespesas" ref="A1:K382" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF54E884-AE1C-4BA9-AAE0-247962D6BA1D}" name="ConsorcioDespesas" displayName="ConsorcioDespesas" ref="A1:K398" totalsRowShown="0">
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{0E4E83A9-3008-4F12-867F-9127FDCBEBC7}" name="consorcio"/>
     <tableColumn id="2" xr3:uid="{AB479D49-5AA3-4445-8011-E951C1F88768}" name="data_base"/>
@@ -1010,10 +1010,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:K382"/>
+  <dimension ref="A1:K398"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A349" workbookViewId="0">
-      <selection activeCell="F383" sqref="F383"/>
+    <sheetView tabSelected="1" topLeftCell="A363" workbookViewId="0">
+      <selection activeCell="F396" sqref="F396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15533,6 +15533,614 @@
         <v>10</v>
       </c>
     </row>
+    <row r="383" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>0</v>
+      </c>
+      <c r="B383" s="4">
+        <v>45657</v>
+      </c>
+      <c r="C383">
+        <v>4</v>
+      </c>
+      <c r="D383">
+        <v>122</v>
+      </c>
+      <c r="E383" s="3">
+        <v>319011010100</v>
+      </c>
+      <c r="F383" s="2">
+        <v>901.39</v>
+      </c>
+      <c r="G383" s="2">
+        <v>901.39</v>
+      </c>
+      <c r="H383" s="2">
+        <v>901.39</v>
+      </c>
+      <c r="I383" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J383" s="1" cm="1">
+        <f t="array" ref="J383">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K383" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="384" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>0</v>
+      </c>
+      <c r="B384" s="4">
+        <v>45657</v>
+      </c>
+      <c r="C384">
+        <v>4</v>
+      </c>
+      <c r="D384">
+        <v>122</v>
+      </c>
+      <c r="E384" s="3">
+        <v>319013010100</v>
+      </c>
+      <c r="F384" s="2">
+        <v>108.4</v>
+      </c>
+      <c r="G384" s="2">
+        <v>108.4</v>
+      </c>
+      <c r="H384" s="2">
+        <v>108.4</v>
+      </c>
+      <c r="I384" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J384" s="1" cm="1">
+        <f t="array" ref="J384">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K384" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>0</v>
+      </c>
+      <c r="B385" s="4">
+        <v>45657</v>
+      </c>
+      <c r="C385">
+        <v>4</v>
+      </c>
+      <c r="D385">
+        <v>122</v>
+      </c>
+      <c r="E385" s="3">
+        <v>319013020100</v>
+      </c>
+      <c r="F385" s="2">
+        <v>378.58</v>
+      </c>
+      <c r="G385" s="2">
+        <v>378.58</v>
+      </c>
+      <c r="H385" s="2">
+        <v>378.58</v>
+      </c>
+      <c r="I385" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J385" s="1" cm="1">
+        <f t="array" ref="J385">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K385" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="386" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>0</v>
+      </c>
+      <c r="B386" s="4">
+        <v>45657</v>
+      </c>
+      <c r="C386">
+        <v>4</v>
+      </c>
+      <c r="D386">
+        <v>122</v>
+      </c>
+      <c r="E386" s="3">
+        <v>339014140000</v>
+      </c>
+      <c r="F386" s="2">
+        <v>0</v>
+      </c>
+      <c r="G386" s="2">
+        <v>0</v>
+      </c>
+      <c r="H386" s="2">
+        <v>0</v>
+      </c>
+      <c r="I386" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J386" s="1" cm="1">
+        <f t="array" ref="J386">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K386" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="387" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>0</v>
+      </c>
+      <c r="B387" s="4">
+        <v>45657</v>
+      </c>
+      <c r="C387">
+        <v>4</v>
+      </c>
+      <c r="D387">
+        <v>122</v>
+      </c>
+      <c r="E387" s="3">
+        <v>339030000000</v>
+      </c>
+      <c r="F387" s="2">
+        <v>0</v>
+      </c>
+      <c r="G387" s="2">
+        <v>0</v>
+      </c>
+      <c r="H387" s="2">
+        <v>0</v>
+      </c>
+      <c r="I387" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J387" s="1" cm="1">
+        <f t="array" ref="J387">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K387" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="388" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>0</v>
+      </c>
+      <c r="B388" s="4">
+        <v>45657</v>
+      </c>
+      <c r="C388">
+        <v>4</v>
+      </c>
+      <c r="D388">
+        <v>122</v>
+      </c>
+      <c r="E388" s="3">
+        <v>339033010000</v>
+      </c>
+      <c r="F388" s="2">
+        <v>0</v>
+      </c>
+      <c r="G388" s="2">
+        <v>0</v>
+      </c>
+      <c r="H388" s="2">
+        <v>0</v>
+      </c>
+      <c r="I388" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J388" s="1" cm="1">
+        <f t="array" ref="J388">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K388" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>0</v>
+      </c>
+      <c r="B389" s="4">
+        <v>45657</v>
+      </c>
+      <c r="C389">
+        <v>4</v>
+      </c>
+      <c r="D389">
+        <v>122</v>
+      </c>
+      <c r="E389" s="3">
+        <v>339039000000</v>
+      </c>
+      <c r="F389" s="2">
+        <v>3.61</v>
+      </c>
+      <c r="G389" s="2">
+        <v>88.69</v>
+      </c>
+      <c r="H389" s="2">
+        <v>130.4</v>
+      </c>
+      <c r="I389" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J389" s="1" cm="1">
+        <f t="array" ref="J389">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K389" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="390" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>0</v>
+      </c>
+      <c r="B390" s="4">
+        <v>45657</v>
+      </c>
+      <c r="C390">
+        <v>4</v>
+      </c>
+      <c r="D390">
+        <v>122</v>
+      </c>
+      <c r="E390" s="3">
+        <v>339039990100</v>
+      </c>
+      <c r="F390" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="G390" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="H390" s="2">
+        <v>59.11</v>
+      </c>
+      <c r="I390" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J390" s="1" cm="1">
+        <f t="array" ref="J390">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K390" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="391" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>0</v>
+      </c>
+      <c r="B391" s="4">
+        <v>45657</v>
+      </c>
+      <c r="C391">
+        <v>4</v>
+      </c>
+      <c r="D391">
+        <v>122</v>
+      </c>
+      <c r="E391" s="3">
+        <v>339039400000</v>
+      </c>
+      <c r="F391" s="2">
+        <v>0</v>
+      </c>
+      <c r="G391" s="2">
+        <v>286.32</v>
+      </c>
+      <c r="H391" s="2">
+        <v>166.83</v>
+      </c>
+      <c r="I391" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J391" s="1" cm="1">
+        <f t="array" ref="J391">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K391" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="392" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>0</v>
+      </c>
+      <c r="B392" s="4">
+        <v>45657</v>
+      </c>
+      <c r="C392">
+        <v>4</v>
+      </c>
+      <c r="D392">
+        <v>122</v>
+      </c>
+      <c r="E392" s="3">
+        <v>339046010100</v>
+      </c>
+      <c r="F392" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="G392" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="H392" s="2">
+        <v>53.48</v>
+      </c>
+      <c r="I392" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J392" s="1" cm="1">
+        <f t="array" ref="J392">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K392" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="393" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>0</v>
+      </c>
+      <c r="B393" s="4">
+        <v>45657</v>
+      </c>
+      <c r="C393">
+        <v>4</v>
+      </c>
+      <c r="D393">
+        <v>122</v>
+      </c>
+      <c r="E393" s="3">
+        <v>339047000000</v>
+      </c>
+      <c r="F393" s="2">
+        <v>0</v>
+      </c>
+      <c r="G393" s="2">
+        <v>0</v>
+      </c>
+      <c r="H393" s="2">
+        <v>0</v>
+      </c>
+      <c r="I393" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J393" s="1" cm="1">
+        <f t="array" ref="J393">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K393" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="394" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>0</v>
+      </c>
+      <c r="B394" s="4">
+        <v>45657</v>
+      </c>
+      <c r="C394">
+        <v>4</v>
+      </c>
+      <c r="D394">
+        <v>122</v>
+      </c>
+      <c r="E394" s="3">
+        <v>339049010000</v>
+      </c>
+      <c r="F394" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="G394" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="H394" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="I394" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J394" s="1" cm="1">
+        <f t="array" ref="J394">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K394" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="395" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>0</v>
+      </c>
+      <c r="B395" s="4">
+        <v>45657</v>
+      </c>
+      <c r="C395">
+        <v>4</v>
+      </c>
+      <c r="D395">
+        <v>122</v>
+      </c>
+      <c r="E395" s="3">
+        <v>449052000000</v>
+      </c>
+      <c r="F395" s="2">
+        <v>190.74</v>
+      </c>
+      <c r="G395" s="2">
+        <v>190.74</v>
+      </c>
+      <c r="H395" s="2">
+        <v>190.74</v>
+      </c>
+      <c r="I395" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J395" s="1" cm="1">
+        <f t="array" ref="J395">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K395" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="396" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>0</v>
+      </c>
+      <c r="B396" s="4">
+        <v>45657</v>
+      </c>
+      <c r="C396">
+        <v>10</v>
+      </c>
+      <c r="D396">
+        <v>302</v>
+      </c>
+      <c r="E396" s="3">
+        <v>334041390500</v>
+      </c>
+      <c r="F396" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="G396" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="H396" s="2">
+        <v>9273.68</v>
+      </c>
+      <c r="I396" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J396" s="1" cm="1">
+        <f t="array" ref="J396">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K396" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="397" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
+        <v>0</v>
+      </c>
+      <c r="B397" s="4">
+        <v>45657</v>
+      </c>
+      <c r="C397">
+        <v>10</v>
+      </c>
+      <c r="D397">
+        <v>302</v>
+      </c>
+      <c r="E397" s="3">
+        <v>334041391100</v>
+      </c>
+      <c r="F397" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="G397" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="H397" s="2">
+        <v>865.54</v>
+      </c>
+      <c r="I397" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J397" s="1" cm="1">
+        <f t="array" ref="J397">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K397" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="398" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
+        <v>0</v>
+      </c>
+      <c r="B398" s="4">
+        <v>45657</v>
+      </c>
+      <c r="C398">
+        <v>10</v>
+      </c>
+      <c r="D398">
+        <v>302</v>
+      </c>
+      <c r="E398" s="3">
+        <v>334041391000</v>
+      </c>
+      <c r="F398" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="G398" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="H398" s="2">
+        <v>655.91</v>
+      </c>
+      <c r="I398" s="1">
+        <f>YEAR(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>2024</v>
+      </c>
+      <c r="J398" s="1" cm="1">
+        <f t="array" ref="J398">_xlfn.SWITCH(MONTH(ConsorcioDespesas[[#This Row],[data_base]]),1,1,2,1,3,2,4,2,5,3,6,3,7,4,8,4,9,5,10,5,11,6,12,6)</f>
+        <v>6</v>
+      </c>
+      <c r="K398" s="1">
+        <f>MONTH(ConsorcioDespesas[[#This Row],[data_base]])</f>
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>